<commit_message>
made new branch timeDate and changed persepctive of changing the timedate
</commit_message>
<xml_diff>
--- a/wedstrijden.xlsx
+++ b/wedstrijden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\handbal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A310541B-F9BD-4B88-A379-D3C8BEE40F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC6DDED-F668-4C38-9314-8633999D30BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2155,8 +2155,8 @@
   <dimension ref="A1:N269"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1" sqref="N1:N1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added try catch statement
</commit_message>
<xml_diff>
--- a/wedstrijden.xlsx
+++ b/wedstrijden.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\handbal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC6DDED-F668-4C38-9314-8633999D30BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F6E252-EC31-4C6B-97B4-DA25C189C031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3645" yWindow="1215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="21-22" sheetId="1" r:id="rId1"/>
@@ -2155,8 +2155,8 @@
   <dimension ref="A1:N269"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D78" sqref="D78"/>
+      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D233" sqref="D233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2210,7 +2210,7 @@
       </c>
       <c r="N1" s="6"/>
     </row>
-    <row r="2" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>131</v>
       </c>
@@ -2240,7 +2240,7 @@
       </c>
       <c r="N2" s="12"/>
     </row>
-    <row r="3" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11969</v>
       </c>
@@ -2270,7 +2270,7 @@
       </c>
       <c r="N3" s="12"/>
     </row>
-    <row r="4" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1477</v>
       </c>
@@ -2300,7 +2300,7 @@
       </c>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11691</v>
       </c>
@@ -2327,7 +2327,7 @@
       <c r="J5" s="7"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>11681</v>
       </c>
@@ -2354,7 +2354,7 @@
       <c r="J6" s="7"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11680</v>
       </c>
@@ -2381,7 +2381,7 @@
       <c r="J7" s="7"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1212</v>
       </c>
@@ -2408,7 +2408,7 @@
       <c r="J8" s="7"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2100</v>
       </c>
@@ -2435,7 +2435,7 @@
       <c r="J9" s="7"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1277</v>
       </c>
@@ -2462,7 +2462,7 @@
       <c r="J10" s="7"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11682</v>
       </c>
@@ -2489,7 +2489,7 @@
       <c r="J11" s="7"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11687</v>
       </c>
@@ -2516,7 +2516,7 @@
       <c r="J12" s="7"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11677</v>
       </c>
@@ -2543,7 +2543,7 @@
       <c r="J13" s="7"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2360</v>
       </c>
@@ -2570,7 +2570,7 @@
       <c r="J14" s="7"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2355</v>
       </c>
@@ -2597,7 +2597,7 @@
       <c r="J15" s="7"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2312</v>
       </c>
@@ -2624,7 +2624,7 @@
       <c r="J16" s="7"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2307</v>
       </c>
@@ -2651,7 +2651,7 @@
       <c r="J17" s="7"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7629</v>
       </c>
@@ -2678,7 +2678,7 @@
       <c r="J18" s="7"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7613</v>
       </c>
@@ -2705,7 +2705,7 @@
       <c r="J19" s="7"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>561</v>
       </c>
@@ -2734,7 +2734,7 @@
       <c r="J20" s="7"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6927</v>
       </c>
@@ -2761,7 +2761,7 @@
       <c r="J21" s="7"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>265</v>
       </c>
@@ -2792,7 +2792,7 @@
       <c r="J22" s="7"/>
       <c r="N22" s="5"/>
     </row>
-    <row r="23" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>1546</v>
       </c>
@@ -2823,7 +2823,7 @@
       <c r="J23" s="7"/>
       <c r="N23" s="5"/>
     </row>
-    <row r="24" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>1418</v>
       </c>
@@ -2854,7 +2854,7 @@
       <c r="J24" s="7"/>
       <c r="N24" s="5"/>
     </row>
-    <row r="25" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>1558</v>
       </c>
@@ -2885,7 +2885,7 @@
       <c r="J25" s="7"/>
       <c r="N25" s="5"/>
     </row>
-    <row r="26" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>1638</v>
       </c>
@@ -2916,7 +2916,7 @@
       <c r="J26" s="7"/>
       <c r="N26" s="5"/>
     </row>
-    <row r="27" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>1910</v>
       </c>
@@ -2947,7 +2947,7 @@
       <c r="J27" s="7"/>
       <c r="N27" s="5"/>
     </row>
-    <row r="28" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>375</v>
       </c>
@@ -2978,7 +2978,7 @@
       <c r="J28" s="7"/>
       <c r="N28" s="5"/>
     </row>
-    <row r="29" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>2042</v>
       </c>
@@ -3009,7 +3009,7 @@
       <c r="J29" s="7"/>
       <c r="N29" s="5"/>
     </row>
-    <row r="30" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>806</v>
       </c>
@@ -3040,7 +3040,7 @@
       <c r="J30" s="7"/>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>2077</v>
       </c>
@@ -3071,7 +3071,7 @@
       <c r="J31" s="7"/>
       <c r="N31" s="5"/>
     </row>
-    <row r="32" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>345</v>
       </c>
@@ -3102,7 +3102,7 @@
       <c r="J32" s="7"/>
       <c r="N32" s="5"/>
     </row>
-    <row r="33" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>11683</v>
       </c>
@@ -3129,7 +3129,7 @@
       <c r="J33" s="7"/>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>11667</v>
       </c>
@@ -3156,7 +3156,7 @@
       <c r="J34" s="7"/>
       <c r="N34" s="2"/>
     </row>
-    <row r="35" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>11395</v>
       </c>
@@ -3183,7 +3183,7 @@
       <c r="J35" s="7"/>
       <c r="N35" s="2"/>
     </row>
-    <row r="36" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>11391</v>
       </c>
@@ -3210,7 +3210,7 @@
       <c r="J36" s="7"/>
       <c r="N36" s="2"/>
     </row>
-    <row r="37" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2575</v>
       </c>
@@ -3243,7 +3243,7 @@
       </c>
       <c r="N37" s="2"/>
     </row>
-    <row r="38" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2569</v>
       </c>
@@ -3276,7 +3276,7 @@
       </c>
       <c r="N38" s="2"/>
     </row>
-    <row r="39" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2525</v>
       </c>
@@ -3309,7 +3309,7 @@
       </c>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>7678</v>
       </c>
@@ -3342,7 +3342,7 @@
       </c>
       <c r="N40" s="2"/>
     </row>
-    <row r="41" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2522</v>
       </c>
@@ -3375,7 +3375,7 @@
       </c>
       <c r="N41" s="2"/>
     </row>
-    <row r="42" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>7695</v>
       </c>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="N42" s="2"/>
     </row>
-    <row r="43" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>766</v>
       </c>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="N43" s="2"/>
     </row>
-    <row r="44" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>6938</v>
       </c>
@@ -3471,7 +3471,7 @@
       </c>
       <c r="N44" s="2"/>
     </row>
-    <row r="45" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2754</v>
       </c>
@@ -3498,7 +3498,7 @@
       <c r="J45" s="7"/>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2741</v>
       </c>
@@ -3525,7 +3525,7 @@
       <c r="J46" s="7"/>
       <c r="N46" s="2"/>
     </row>
-    <row r="47" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>12527</v>
       </c>
@@ -3555,7 +3555,7 @@
       </c>
       <c r="N47" s="2"/>
     </row>
-    <row r="48" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>7781</v>
       </c>
@@ -3586,7 +3586,7 @@
       </c>
       <c r="N48" s="2"/>
     </row>
-    <row r="49" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2665</v>
       </c>
@@ -3613,7 +3613,7 @@
       <c r="J49" s="7"/>
       <c r="N49" s="2"/>
     </row>
-    <row r="50" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1009</v>
       </c>
@@ -3644,7 +3644,7 @@
       </c>
       <c r="N50" s="2"/>
     </row>
-    <row r="51" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>10255</v>
       </c>
@@ -3671,7 +3671,7 @@
       <c r="J51" s="7"/>
       <c r="N51" s="2"/>
     </row>
-    <row r="52" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1400</v>
       </c>
@@ -3700,7 +3700,7 @@
       </c>
       <c r="N52" s="2"/>
     </row>
-    <row r="53" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1572</v>
       </c>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="N53" s="2"/>
     </row>
-    <row r="54" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1729</v>
       </c>
@@ -3758,7 +3758,7 @@
       </c>
       <c r="N54" s="2"/>
     </row>
-    <row r="55" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>13171</v>
       </c>
@@ -3790,7 +3790,7 @@
       </c>
       <c r="N55" s="2"/>
     </row>
-    <row r="56" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>13218</v>
       </c>
@@ -3822,7 +3822,7 @@
       </c>
       <c r="N56" s="10"/>
     </row>
-    <row r="57" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>13252</v>
       </c>
@@ -3854,7 +3854,7 @@
       </c>
       <c r="N57" s="2"/>
     </row>
-    <row r="58" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>7814</v>
       </c>
@@ -3881,7 +3881,7 @@
       <c r="J58" s="7"/>
       <c r="N58" s="2"/>
     </row>
-    <row r="59" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2965</v>
       </c>
@@ -3914,7 +3914,7 @@
       </c>
       <c r="N59" s="2"/>
     </row>
-    <row r="60" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2959</v>
       </c>
@@ -3947,7 +3947,7 @@
       </c>
       <c r="N60" s="2"/>
     </row>
-    <row r="61" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2918</v>
       </c>
@@ -3980,7 +3980,7 @@
       </c>
       <c r="N61" s="2"/>
     </row>
-    <row r="62" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2915</v>
       </c>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="N62" s="2"/>
     </row>
-    <row r="63" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1179</v>
       </c>
@@ -4045,7 +4045,7 @@
       </c>
       <c r="N63" s="10"/>
     </row>
-    <row r="64" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>3128</v>
       </c>
@@ -4072,7 +4072,7 @@
       <c r="J64" s="7"/>
       <c r="N64" s="2"/>
     </row>
-    <row r="65" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>3075</v>
       </c>
@@ -4099,7 +4099,7 @@
       <c r="J65" s="7"/>
       <c r="N65" s="2"/>
     </row>
-    <row r="66" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>7881</v>
       </c>
@@ -4132,7 +4132,7 @@
       </c>
       <c r="N66" s="2"/>
     </row>
-    <row r="67" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>7897</v>
       </c>
@@ -4163,7 +4163,7 @@
       </c>
       <c r="N67" s="2"/>
     </row>
-    <row r="68" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1416</v>
       </c>
@@ -4194,7 +4194,7 @@
       </c>
       <c r="N68" s="2"/>
     </row>
-    <row r="69" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>3125</v>
       </c>
@@ -4221,7 +4221,7 @@
       <c r="J69" s="7"/>
       <c r="N69" s="2"/>
     </row>
-    <row r="70" spans="1:14" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="26">
         <v>7830</v>
       </c>
@@ -4251,7 +4251,7 @@
       </c>
       <c r="N70" s="10"/>
     </row>
-    <row r="71" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="18">
         <v>3405</v>
       </c>
@@ -4287,7 +4287,7 @@
       </c>
       <c r="N71" s="10"/>
     </row>
-    <row r="72" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="18">
         <v>3399</v>
       </c>
@@ -4323,7 +4323,7 @@
       </c>
       <c r="N72" s="10"/>
     </row>
-    <row r="73" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="18">
         <v>3316</v>
       </c>
@@ -4359,7 +4359,7 @@
       </c>
       <c r="N73" s="10"/>
     </row>
-    <row r="74" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="18">
         <v>3313</v>
       </c>
@@ -4392,7 +4392,7 @@
       </c>
       <c r="N74" s="10"/>
     </row>
-    <row r="75" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>7981</v>
       </c>
@@ -4419,7 +4419,7 @@
       <c r="J75" s="7"/>
       <c r="N75" s="2"/>
     </row>
-    <row r="76" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>7966</v>
       </c>
@@ -4449,7 +4449,7 @@
       </c>
       <c r="N76" s="2"/>
     </row>
-    <row r="77" spans="1:14" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1658</v>
       </c>

</xml_diff>

<commit_message>
added spatie bij datum en tijd
</commit_message>
<xml_diff>
--- a/wedstrijden.xlsx
+++ b/wedstrijden.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\handbal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F6E252-EC31-4C6B-97B4-DA25C189C031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE8A3B9-5F4E-4A3D-8F12-80B149332D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="1215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="21-22" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <author>Rodijk, Peter</author>
   </authors>
   <commentList>
-    <comment ref="D101" authorId="0" shapeId="0" xr:uid="{AB520BB5-CD8E-4FB7-8133-CC68E2B4D17E}">
+    <comment ref="C101" authorId="0" shapeId="0" xr:uid="{F9A7DAE8-1CC9-4A61-B951-69184ED17577}">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N101" authorId="0" shapeId="0" xr:uid="{877AF1D6-C38D-441E-89A2-FE7F3F9822CE}">
+    <comment ref="N101" authorId="0" shapeId="0" xr:uid="{48EB4A89-B750-4526-BE20-7EC2BA436B0D}">
       <text>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D102" authorId="0" shapeId="0" xr:uid="{9241C55E-D40E-426C-BD28-7AF9D9AB34DF}">
+    <comment ref="C102" authorId="0" shapeId="0" xr:uid="{817CBE2D-1037-4740-A75B-65F7012BA2FC}">
       <text>
         <r>
           <rPr>
@@ -108,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N102" authorId="0" shapeId="0" xr:uid="{EDF9BA67-246C-443B-A073-D2FD3A3E1F46}">
+    <comment ref="N102" authorId="0" shapeId="0" xr:uid="{F6E62098-B102-47C8-AB03-22D9C18CCA53}">
       <text>
         <r>
           <rPr>
@@ -132,7 +132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D103" authorId="0" shapeId="0" xr:uid="{6EE115B3-879C-4E14-A3DF-9587C3282E0C}">
+    <comment ref="C103" authorId="0" shapeId="0" xr:uid="{CCC1B6BF-3F2D-4319-A858-B36D36F4A098}">
       <text>
         <r>
           <rPr>
@@ -156,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N103" authorId="0" shapeId="0" xr:uid="{47CDA934-8918-4A10-ACFA-640B7A7DB798}">
+    <comment ref="N103" authorId="0" shapeId="0" xr:uid="{6D00A083-A871-4EC4-B0CD-15F5438BAB27}">
       <text>
         <r>
           <rPr>
@@ -180,7 +180,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D104" authorId="0" shapeId="0" xr:uid="{F7050025-5627-47DF-93FC-8E527DC36CAE}">
+    <comment ref="C104" authorId="0" shapeId="0" xr:uid="{234FC450-6F1C-4D4E-AC53-677B6956D5BA}">
       <text>
         <r>
           <rPr>
@@ -204,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N104" authorId="0" shapeId="0" xr:uid="{08B5DC8C-1355-4BE7-AA38-22966EA4CE79}">
+    <comment ref="N104" authorId="0" shapeId="0" xr:uid="{629F546C-1DB0-44EB-B8D7-B043BF89095E}">
       <text>
         <r>
           <rPr>
@@ -2155,15 +2155,14 @@
   <dimension ref="A1:N269"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D233" sqref="D233"/>
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.140625" style="8" customWidth="1"/>
@@ -2171,6 +2170,7 @@
     <col min="10" max="10" width="31" style="8" customWidth="1"/>
     <col min="11" max="11" width="20.140625" style="11" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2182,10 +2182,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>4</v>
@@ -2208,6 +2208,7 @@
       <c r="K1" s="16" t="s">
         <v>206</v>
       </c>
+      <c r="M1" s="6"/>
       <c r="N1" s="6"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2217,11 +2218,11 @@
       <c r="B2" s="1">
         <v>44450</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="12">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="12">
-        <v>0.3888888888888889</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -2247,11 +2248,11 @@
       <c r="B3" s="1">
         <v>44450</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="12">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0.40277777777777773</v>
       </c>
       <c r="E3" t="s">
         <v>21</v>
@@ -2277,11 +2278,11 @@
       <c r="B4" s="1">
         <v>44450</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.43055555555555558</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -2307,11 +2308,11 @@
       <c r="B5" s="1">
         <v>44450</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2">
+        <v>0.46875</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.46875</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -2334,11 +2335,11 @@
       <c r="B6" s="1">
         <v>44450</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.50347222222222221</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
@@ -2361,11 +2362,11 @@
       <c r="B7" s="1">
         <v>44450</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D7" t="s">
         <v>14</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.52083333333333337</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
@@ -2388,11 +2389,11 @@
       <c r="B8" s="1">
         <v>44464</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D8" t="s">
         <v>17</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.3888888888888889</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -2415,11 +2416,11 @@
       <c r="B9" s="1">
         <v>44464</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D9" t="s">
         <v>20</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -2442,11 +2443,11 @@
       <c r="B10" s="1">
         <v>44464</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D10" t="s">
         <v>7</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.43055555555555558</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
@@ -2469,11 +2470,11 @@
       <c r="B11" s="1">
         <v>44464</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D11" t="s">
         <v>14</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.4375</v>
       </c>
       <c r="E11" t="s">
         <v>22</v>
@@ -2496,11 +2497,11 @@
       <c r="B12" s="1">
         <v>44464</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="D12" t="s">
         <v>16</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.4513888888888889</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
@@ -2523,11 +2524,11 @@
       <c r="B13" s="1">
         <v>44464</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D13" t="s">
         <v>25</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0.47916666666666669</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -2550,11 +2551,11 @@
       <c r="B14" s="1">
         <v>44471</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="D14" t="s">
         <v>26</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.41319444444444442</v>
       </c>
       <c r="E14" t="s">
         <v>27</v>
@@ -2577,11 +2578,11 @@
       <c r="B15" s="1">
         <v>44471</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2">
+        <v>0.59375</v>
+      </c>
+      <c r="D15" t="s">
         <v>29</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.59375</v>
       </c>
       <c r="E15" t="s">
         <v>30</v>
@@ -2604,11 +2605,11 @@
       <c r="B16" s="1">
         <v>44471</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D16" t="s">
         <v>33</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.69791666666666663</v>
       </c>
       <c r="E16" t="s">
         <v>34</v>
@@ -2631,11 +2632,11 @@
       <c r="B17" s="1">
         <v>44471</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D17" t="s">
         <v>35</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0.75</v>
       </c>
       <c r="E17" t="s">
         <v>36</v>
@@ -2658,11 +2659,11 @@
       <c r="B18" s="1">
         <v>44472</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D18" t="s">
         <v>39</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E18" t="s">
         <v>40</v>
@@ -2685,11 +2686,11 @@
       <c r="B19" s="1">
         <v>44472</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D19" t="s">
         <v>43</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E19" t="s">
         <v>44</v>
@@ -2712,11 +2713,11 @@
       <c r="B20" s="1">
         <v>44472</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D20" t="s">
         <v>45</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.52083333333333337</v>
       </c>
       <c r="E20" t="s">
         <v>46</v>
@@ -2741,11 +2742,11 @@
       <c r="B21" s="1">
         <v>44474</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="D21" t="s">
         <v>47</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0.875</v>
       </c>
       <c r="E21" t="s">
         <v>48</v>
@@ -2768,11 +2769,11 @@
       <c r="B22" s="4">
         <v>44478</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="D22" s="5">
-        <v>0.375</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>17</v>
@@ -2790,6 +2791,7 @@
         <v>197</v>
       </c>
       <c r="J22" s="7"/>
+      <c r="M22" s="3"/>
       <c r="N22" s="5"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -2799,11 +2801,11 @@
       <c r="B23" s="4">
         <v>44478</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="D23" s="5">
-        <v>0.375</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>7</v>
@@ -2821,6 +2823,7 @@
         <v>199</v>
       </c>
       <c r="J23" s="7"/>
+      <c r="M23" s="3"/>
       <c r="N23" s="5"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -2830,11 +2833,11 @@
       <c r="B24" s="4">
         <v>44478</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="5">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="D24" s="5">
-        <v>0.3888888888888889</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>8</v>
@@ -2852,6 +2855,7 @@
         <v>201</v>
       </c>
       <c r="J24" s="7"/>
+      <c r="M24" s="3"/>
       <c r="N24" s="5"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -2861,11 +2865,11 @@
       <c r="B25" s="4">
         <v>44478</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="5">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="D25" s="5">
-        <v>0.3888888888888889</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>20</v>
@@ -2883,6 +2887,7 @@
         <v>203</v>
       </c>
       <c r="J25" s="7"/>
+      <c r="M25" s="3"/>
       <c r="N25" s="5"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -2892,11 +2897,11 @@
       <c r="B26" s="4">
         <v>44478</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="5">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D26" s="5">
-        <v>0.40277777777777773</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>12</v>
@@ -2914,6 +2919,7 @@
         <v>197</v>
       </c>
       <c r="J26" s="7"/>
+      <c r="M26" s="3"/>
       <c r="N26" s="5"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -2923,11 +2929,11 @@
       <c r="B27" s="4">
         <v>44478</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="5">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D27" s="5">
-        <v>0.40277777777777773</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>11</v>
@@ -2945,6 +2951,7 @@
         <v>199</v>
       </c>
       <c r="J27" s="7"/>
+      <c r="M27" s="3"/>
       <c r="N27" s="5"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -2954,11 +2961,11 @@
       <c r="B28" s="4">
         <v>44478</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="D28" s="5">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>8</v>
@@ -2976,6 +2983,7 @@
         <v>201</v>
       </c>
       <c r="J28" s="7"/>
+      <c r="M28" s="3"/>
       <c r="N28" s="5"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -2985,11 +2993,11 @@
       <c r="B29" s="4">
         <v>44478</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="D29" s="5">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>21</v>
@@ -3007,6 +3015,7 @@
         <v>203</v>
       </c>
       <c r="J29" s="7"/>
+      <c r="M29" s="3"/>
       <c r="N29" s="5"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -3016,11 +3025,11 @@
       <c r="B30" s="4">
         <v>44478</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="5">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="D30" s="5">
-        <v>0.43055555555555558</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>7</v>
@@ -3038,6 +3047,7 @@
         <v>197</v>
       </c>
       <c r="J30" s="7"/>
+      <c r="M30" s="3"/>
       <c r="N30" s="5"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -3047,11 +3057,11 @@
       <c r="B31" s="4">
         <v>44478</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="5">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D31" s="5">
-        <v>0.43055555555555558</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>20</v>
@@ -3069,6 +3079,7 @@
         <v>199</v>
       </c>
       <c r="J31" s="7"/>
+      <c r="M31" s="3"/>
       <c r="N31" s="5"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -3078,11 +3089,11 @@
       <c r="B32" s="4">
         <v>44478</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="5">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="D32" s="5">
-        <v>0.44444444444444442</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>12</v>
@@ -3100,6 +3111,7 @@
         <v>201</v>
       </c>
       <c r="J32" s="7"/>
+      <c r="M32" s="3"/>
       <c r="N32" s="5"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -3109,11 +3121,11 @@
       <c r="B33" s="1">
         <v>44478</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D33" t="s">
         <v>14</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0.375</v>
       </c>
       <c r="E33" t="s">
         <v>25</v>
@@ -3136,11 +3148,11 @@
       <c r="B34" s="1">
         <v>44478</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D34" t="s">
         <v>22</v>
-      </c>
-      <c r="D34" s="2">
-        <v>0.3888888888888889</v>
       </c>
       <c r="E34" t="s">
         <v>14</v>
@@ -3163,11 +3175,11 @@
       <c r="B35" s="1">
         <v>44478</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D35" t="s">
         <v>13</v>
-      </c>
-      <c r="D35" s="2">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E35" t="s">
         <v>14</v>
@@ -3190,11 +3202,11 @@
       <c r="B36" s="1">
         <v>44478</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D36" t="s">
         <v>14</v>
-      </c>
-      <c r="D36" s="2">
-        <v>0.43055555555555558</v>
       </c>
       <c r="E36" t="s">
         <v>16</v>
@@ -3217,11 +3229,11 @@
       <c r="B37" s="1">
         <v>44478</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="D37" t="s">
         <v>27</v>
-      </c>
-      <c r="D37" s="2">
-        <v>0.55555555555555558</v>
       </c>
       <c r="E37" t="s">
         <v>53</v>
@@ -3250,11 +3262,11 @@
       <c r="B38" s="1">
         <v>44478</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2">
+        <v>0.59375</v>
+      </c>
+      <c r="D38" t="s">
         <v>30</v>
-      </c>
-      <c r="D38" s="2">
-        <v>0.59375</v>
       </c>
       <c r="E38" t="s">
         <v>54</v>
@@ -3283,11 +3295,11 @@
       <c r="B39" s="1">
         <v>44478</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D39" t="s">
         <v>34</v>
-      </c>
-      <c r="D39" s="2">
-        <v>0.625</v>
       </c>
       <c r="E39" t="s">
         <v>55</v>
@@ -3316,11 +3328,11 @@
       <c r="B40" s="1">
         <v>44478</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D40" t="s">
         <v>44</v>
-      </c>
-      <c r="D40" s="2">
-        <v>0.66666666666666663</v>
       </c>
       <c r="E40" t="s">
         <v>56</v>
@@ -3349,11 +3361,11 @@
       <c r="B41" s="1">
         <v>44478</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D41" t="s">
         <v>36</v>
-      </c>
-      <c r="D41" s="2">
-        <v>0.70833333333333337</v>
       </c>
       <c r="E41" t="s">
         <v>57</v>
@@ -3382,11 +3394,11 @@
       <c r="B42" s="1">
         <v>44478</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D42" t="s">
         <v>40</v>
-      </c>
-      <c r="D42" s="2">
-        <v>0.75</v>
       </c>
       <c r="E42" t="s">
         <v>58</v>
@@ -3413,11 +3425,11 @@
       <c r="B43" s="1">
         <v>44478</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="2">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D43" t="s">
         <v>46</v>
-      </c>
-      <c r="D43" s="2">
-        <v>0.82291666666666663</v>
       </c>
       <c r="E43" t="s">
         <v>59</v>
@@ -3444,11 +3456,11 @@
       <c r="B44" s="1">
         <v>44482</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="2">
+        <v>0.84375</v>
+      </c>
+      <c r="D44" t="s">
         <v>48</v>
-      </c>
-      <c r="D44" s="2">
-        <v>0.84375</v>
       </c>
       <c r="E44" t="s">
         <v>60</v>
@@ -3478,11 +3490,11 @@
       <c r="B45" s="1">
         <v>44485</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D45" t="s">
         <v>61</v>
-      </c>
-      <c r="D45" s="2">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E45" t="s">
         <v>27</v>
@@ -3505,11 +3517,11 @@
       <c r="B46" s="1">
         <v>44485</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D46" t="s">
         <v>64</v>
-      </c>
-      <c r="D46" s="2">
-        <v>0.66666666666666663</v>
       </c>
       <c r="E46" t="s">
         <v>30</v>
@@ -3532,11 +3544,11 @@
       <c r="B47" s="1">
         <v>44485</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="2">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D47" t="s">
         <v>295</v>
-      </c>
-      <c r="D47" s="2">
-        <v>0.69791666666666663</v>
       </c>
       <c r="E47" t="s">
         <v>36</v>
@@ -3562,11 +3574,11 @@
       <c r="B48" s="1">
         <v>44485</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D48" t="s">
         <v>40</v>
-      </c>
-      <c r="D48" s="2">
-        <v>0.75</v>
       </c>
       <c r="E48" t="s">
         <v>70</v>
@@ -3593,11 +3605,11 @@
       <c r="B49" s="1">
         <v>44485</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D49" t="s">
         <v>71</v>
-      </c>
-      <c r="D49" s="2">
-        <v>0.77083333333333337</v>
       </c>
       <c r="E49" t="s">
         <v>34</v>
@@ -3620,11 +3632,11 @@
       <c r="B50" s="1">
         <v>44485</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="2">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D50" t="s">
         <v>46</v>
-      </c>
-      <c r="D50" s="2">
-        <v>0.82291666666666663</v>
       </c>
       <c r="E50" t="s">
         <v>74</v>
@@ -3651,11 +3663,11 @@
       <c r="B51" s="1">
         <v>44496</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D51" t="s">
         <v>75</v>
-      </c>
-      <c r="D51" s="2">
-        <v>0.83333333333333337</v>
       </c>
       <c r="E51" t="s">
         <v>48</v>
@@ -3678,11 +3690,11 @@
       <c r="B52" s="1">
         <v>44499</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D52" t="s">
         <v>7</v>
-      </c>
-      <c r="D52" s="2">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E52" t="s">
         <v>17</v>
@@ -3707,11 +3719,11 @@
       <c r="B53" s="1">
         <v>44499</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="2">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D53" t="s">
         <v>7</v>
-      </c>
-      <c r="D53" s="2">
-        <v>0.44444444444444442</v>
       </c>
       <c r="E53" t="s">
         <v>20</v>
@@ -3736,11 +3748,11 @@
       <c r="B54" s="1">
         <v>44499</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="2">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="D54" t="s">
         <v>21</v>
-      </c>
-      <c r="D54" s="2">
-        <v>0.47222222222222227</v>
       </c>
       <c r="E54" t="s">
         <v>7</v>
@@ -3765,11 +3777,11 @@
       <c r="B55" s="1">
         <v>44499</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D55" t="s">
         <v>22</v>
-      </c>
-      <c r="D55" s="2">
-        <v>0.52083333333333337</v>
       </c>
       <c r="E55" t="s">
         <v>14</v>
@@ -3797,11 +3809,11 @@
       <c r="B56" s="1">
         <v>44499</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="10">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="D56" t="s">
         <v>14</v>
-      </c>
-      <c r="D56" s="10">
-        <v>0.54861111111111105</v>
       </c>
       <c r="E56" t="s">
         <v>16</v>
@@ -3829,11 +3841,11 @@
       <c r="B57" s="1">
         <v>44499</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="D57" t="s">
         <v>13</v>
-      </c>
-      <c r="D57" s="2">
-        <v>0.5625</v>
       </c>
       <c r="E57" t="s">
         <v>14</v>
@@ -3861,11 +3873,11 @@
       <c r="B58" s="1">
         <v>44499</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="2">
+        <v>0.53125</v>
+      </c>
+      <c r="D58" t="s">
         <v>80</v>
-      </c>
-      <c r="D58" s="2">
-        <v>0.53125</v>
       </c>
       <c r="E58" t="s">
         <v>44</v>
@@ -3888,11 +3900,11 @@
       <c r="B59" s="1">
         <v>44499</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="2">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="D59" t="s">
         <v>27</v>
-      </c>
-      <c r="D59" s="2">
-        <v>0.59722222222222221</v>
       </c>
       <c r="E59" t="s">
         <v>83</v>
@@ -3921,11 +3933,11 @@
       <c r="B60" s="1">
         <v>44499</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="2">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D60" t="s">
         <v>30</v>
-      </c>
-      <c r="D60" s="2">
-        <v>0.63541666666666663</v>
       </c>
       <c r="E60" t="s">
         <v>84</v>
@@ -3954,11 +3966,11 @@
       <c r="B61" s="1">
         <v>44499</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D61" t="s">
         <v>34</v>
-      </c>
-      <c r="D61" s="2">
-        <v>0.66666666666666663</v>
       </c>
       <c r="E61" t="s">
         <v>85</v>
@@ -3987,11 +3999,11 @@
       <c r="B62" s="1">
         <v>44499</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D62" t="s">
         <v>36</v>
-      </c>
-      <c r="D62" s="2">
-        <v>0.70833333333333337</v>
       </c>
       <c r="E62" t="s">
         <v>86</v>
@@ -4020,11 +4032,11 @@
       <c r="B63" s="9">
         <v>44499</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="10">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D63" t="s">
         <v>88</v>
-      </c>
-      <c r="D63" s="10">
-        <v>0.79166666666666663</v>
       </c>
       <c r="E63" t="s">
         <v>46</v>
@@ -4052,11 +4064,11 @@
       <c r="B64" s="1">
         <v>44506</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="2">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="D64" t="s">
         <v>91</v>
-      </c>
-      <c r="D64" s="2">
-        <v>0.47569444444444442</v>
       </c>
       <c r="E64" t="s">
         <v>34</v>
@@ -4079,11 +4091,11 @@
       <c r="B65" s="1">
         <v>44506</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="2">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="D65" t="s">
         <v>92</v>
-      </c>
-      <c r="D65" s="2">
-        <v>0.54861111111111105</v>
       </c>
       <c r="E65" t="s">
         <v>27</v>
@@ -4106,11 +4118,11 @@
       <c r="B66" s="1">
         <v>44506</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D66" t="s">
         <v>44</v>
-      </c>
-      <c r="D66" s="2">
-        <v>0.70833333333333337</v>
       </c>
       <c r="E66" t="s">
         <v>95</v>
@@ -4139,11 +4151,11 @@
       <c r="B67" s="1">
         <v>44506</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D67" t="s">
         <v>40</v>
-      </c>
-      <c r="D67" s="2">
-        <v>0.75</v>
       </c>
       <c r="E67" t="s">
         <v>96</v>
@@ -4170,11 +4182,11 @@
       <c r="B68" s="1">
         <v>44506</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="2">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D68" t="s">
         <v>46</v>
-      </c>
-      <c r="D68" s="2">
-        <v>0.82291666666666663</v>
       </c>
       <c r="E68" t="s">
         <v>97</v>
@@ -4201,11 +4213,11 @@
       <c r="B69" s="1">
         <v>44507</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D69" t="s">
         <v>98</v>
-      </c>
-      <c r="D69" s="2">
-        <v>0.5</v>
       </c>
       <c r="E69" t="s">
         <v>36</v>
@@ -4228,11 +4240,11 @@
       <c r="B70" s="1">
         <v>44510</v>
       </c>
-      <c r="C70" s="26" t="s">
+      <c r="C70" s="10">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D70" s="26" t="s">
         <v>87</v>
-      </c>
-      <c r="D70" s="10">
-        <v>0.85416666666666663</v>
       </c>
       <c r="E70" s="26" t="s">
         <v>40</v>
@@ -4258,11 +4270,11 @@
       <c r="B71" s="17">
         <v>44513</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="C71" s="10">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="D71" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="D71" s="10">
-        <v>0.4826388888888889</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>99</v>
@@ -4285,6 +4297,7 @@
       <c r="K71" s="21" t="s">
         <v>303</v>
       </c>
+      <c r="M71" s="8"/>
       <c r="N71" s="10"/>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
@@ -4294,11 +4307,11 @@
       <c r="B72" s="17">
         <v>44513</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="C72" s="10">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D72" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="D72" s="10">
-        <v>0.52083333333333337</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>100</v>
@@ -4321,6 +4334,7 @@
       <c r="K72" s="11" t="s">
         <v>292</v>
       </c>
+      <c r="M72" s="8"/>
       <c r="N72" s="10"/>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
@@ -4330,11 +4344,11 @@
       <c r="B73" s="9">
         <v>44513</v>
       </c>
-      <c r="C73" s="8" t="s">
+      <c r="C73" s="10">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D73" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="D73" s="10">
-        <v>0.66666666666666663</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>101</v>
@@ -4357,6 +4371,7 @@
       <c r="K73" s="11" t="s">
         <v>318</v>
       </c>
+      <c r="M73" s="8"/>
       <c r="N73" s="10"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
@@ -4366,11 +4381,11 @@
       <c r="B74" s="9">
         <v>44513</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="C74" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D74" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="D74" s="10">
-        <v>0.70833333333333337</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>102</v>
@@ -4390,6 +4405,7 @@
       <c r="J74" s="14" t="s">
         <v>229</v>
       </c>
+      <c r="M74" s="8"/>
       <c r="N74" s="10"/>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
@@ -4399,11 +4415,11 @@
       <c r="B75" s="1">
         <v>44514</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D75" t="s">
         <v>103</v>
-      </c>
-      <c r="D75" s="2">
-        <v>0.4375</v>
       </c>
       <c r="E75" t="s">
         <v>40</v>
@@ -4426,11 +4442,11 @@
       <c r="B76" s="1">
         <v>44514</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D76" t="s">
         <v>106</v>
-      </c>
-      <c r="D76" s="2">
-        <v>0.5</v>
       </c>
       <c r="E76" t="s">
         <v>44</v>
@@ -4456,11 +4472,11 @@
       <c r="B77" s="1">
         <v>44514</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D77" t="s">
         <v>107</v>
-      </c>
-      <c r="D77" s="2">
-        <v>0.54166666666666663</v>
       </c>
       <c r="E77" t="s">
         <v>46</v>
@@ -4485,11 +4501,11 @@
       <c r="B78" s="4">
         <v>44520</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C78" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="D78" s="5">
-        <v>0.375</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>13</v>
@@ -4513,7 +4529,7 @@
         <v>308</v>
       </c>
       <c r="L78" s="1"/>
-      <c r="M78" s="2"/>
+      <c r="M78" s="3"/>
       <c r="N78" s="5"/>
     </row>
     <row r="79" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4523,11 +4539,11 @@
       <c r="B79" s="4">
         <v>44520</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C79" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D79" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="D79" s="5">
-        <v>0.375</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>25</v>
@@ -4549,7 +4565,7 @@
       </c>
       <c r="K79"/>
       <c r="L79" s="1"/>
-      <c r="M79" s="2"/>
+      <c r="M79" s="3"/>
       <c r="N79" s="5"/>
     </row>
     <row r="80" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4559,11 +4575,11 @@
       <c r="B80" s="4">
         <v>44520</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C80" s="5">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D80" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="D80" s="5">
-        <v>0.3888888888888889</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>307</v>
@@ -4585,7 +4601,7 @@
       </c>
       <c r="K80"/>
       <c r="L80" s="1"/>
-      <c r="M80" s="2"/>
+      <c r="M80" s="3"/>
       <c r="N80" s="5"/>
     </row>
     <row r="81" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4595,11 +4611,11 @@
       <c r="B81" s="4">
         <v>44520</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C81" s="5">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D81" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="D81" s="5">
-        <v>0.3888888888888889</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>15</v>
@@ -4621,7 +4637,7 @@
       </c>
       <c r="K81"/>
       <c r="L81" s="1"/>
-      <c r="M81" s="2"/>
+      <c r="M81" s="3"/>
       <c r="N81" s="5"/>
     </row>
     <row r="82" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4631,11 +4647,11 @@
       <c r="B82" s="4">
         <v>44520</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C82" s="5">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D82" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D82" s="5">
-        <v>0.40277777777777773</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>22</v>
@@ -4657,7 +4673,7 @@
       </c>
       <c r="K82"/>
       <c r="L82" s="1"/>
-      <c r="M82" s="2"/>
+      <c r="M82" s="3"/>
       <c r="N82" s="5"/>
     </row>
     <row r="83" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4667,11 +4683,11 @@
       <c r="B83" s="4">
         <v>44520</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C83" s="5">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D83" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D83" s="5">
-        <v>0.40277777777777773</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>16</v>
@@ -4693,7 +4709,7 @@
       </c>
       <c r="K83"/>
       <c r="L83" s="1"/>
-      <c r="M83" s="2"/>
+      <c r="M83" s="3"/>
       <c r="N83" s="5"/>
     </row>
     <row r="84" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4703,11 +4719,11 @@
       <c r="B84" s="4">
         <v>44520</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C84" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D84" s="3" t="s">
         <v>307</v>
-      </c>
-      <c r="D84" s="5">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>14</v>
@@ -4729,7 +4745,7 @@
       </c>
       <c r="K84"/>
       <c r="L84" s="1"/>
-      <c r="M84" s="2"/>
+      <c r="M84" s="3"/>
       <c r="N84" s="5"/>
     </row>
     <row r="85" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4739,11 +4755,11 @@
       <c r="B85" s="4">
         <v>44520</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C85" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D85" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D85" s="5">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>25</v>
@@ -4765,7 +4781,7 @@
       </c>
       <c r="K85"/>
       <c r="L85" s="1"/>
-      <c r="M85" s="2"/>
+      <c r="M85" s="3"/>
       <c r="N85" s="5"/>
     </row>
     <row r="86" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4775,11 +4791,11 @@
       <c r="B86" s="4">
         <v>44520</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="C86" s="5">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D86" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="D86" s="5">
-        <v>0.43055555555555558</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>14</v>
@@ -4801,7 +4817,7 @@
       </c>
       <c r="K86"/>
       <c r="L86" s="1"/>
-      <c r="M86" s="2"/>
+      <c r="M86" s="3"/>
       <c r="N86" s="5"/>
     </row>
     <row r="87" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4811,11 +4827,11 @@
       <c r="B87" s="4">
         <v>44520</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C87" s="5">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D87" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="D87" s="5">
-        <v>0.43055555555555558</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>15</v>
@@ -4837,7 +4853,7 @@
       </c>
       <c r="K87"/>
       <c r="L87" s="1"/>
-      <c r="M87" s="2"/>
+      <c r="M87" s="3"/>
       <c r="N87" s="5"/>
     </row>
     <row r="88" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4847,11 +4863,11 @@
       <c r="B88" s="4">
         <v>44520</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C88" s="5">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D88" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="D88" s="5">
-        <v>0.44444444444444442</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>307</v>
@@ -4873,7 +4889,7 @@
       </c>
       <c r="K88"/>
       <c r="L88" s="1"/>
-      <c r="M88" s="2"/>
+      <c r="M88" s="3"/>
       <c r="N88" s="5"/>
     </row>
     <row r="89" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4883,11 +4899,11 @@
       <c r="B89" s="1">
         <v>44520</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D89" t="s">
         <v>108</v>
-      </c>
-      <c r="D89" s="10">
-        <v>0.5</v>
       </c>
       <c r="E89" t="s">
         <v>30</v>
@@ -4910,11 +4926,11 @@
       <c r="B90" s="9">
         <v>44520</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="10">
+        <v>0.59375</v>
+      </c>
+      <c r="D90" t="s">
         <v>109</v>
-      </c>
-      <c r="D90" s="10">
-        <v>0.59375</v>
       </c>
       <c r="E90" t="s">
         <v>27</v>
@@ -4940,11 +4956,11 @@
       <c r="B91" s="1">
         <v>44520</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D91" t="s">
         <v>34</v>
-      </c>
-      <c r="D91" s="2">
-        <v>0.625</v>
       </c>
       <c r="E91" t="s">
         <v>286</v>
@@ -4976,11 +4992,11 @@
       <c r="B92" s="1">
         <v>44520</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D92" t="s">
         <v>44</v>
-      </c>
-      <c r="D92" s="2">
-        <v>0.66666666666666663</v>
       </c>
       <c r="E92" t="s">
         <v>112</v>
@@ -5012,11 +5028,11 @@
       <c r="B93" s="1">
         <v>44520</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D93" t="s">
         <v>36</v>
-      </c>
-      <c r="D93" s="2">
-        <v>0.70833333333333337</v>
       </c>
       <c r="E93" t="s">
         <v>113</v>
@@ -5045,11 +5061,11 @@
       <c r="B94" s="1">
         <v>44520</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D94" t="s">
         <v>40</v>
-      </c>
-      <c r="D94" s="2">
-        <v>0.75</v>
       </c>
       <c r="E94" t="s">
         <v>114</v>
@@ -5076,11 +5092,11 @@
       <c r="B95" s="1">
         <v>44520</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="2">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D95" t="s">
         <v>46</v>
-      </c>
-      <c r="D95" s="2">
-        <v>0.82291666666666663</v>
       </c>
       <c r="E95" t="s">
         <v>115</v>
@@ -5107,11 +5123,11 @@
       <c r="B96" s="1">
         <v>44521</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D96" t="s">
         <v>7</v>
-      </c>
-      <c r="D96" s="2">
-        <v>0.45833333333333331</v>
       </c>
       <c r="E96" t="s">
         <v>8</v>
@@ -5136,11 +5152,11 @@
       <c r="B97" s="1">
         <v>44521</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="2">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="D97" t="s">
         <v>11</v>
-      </c>
-      <c r="D97" s="2">
-        <v>0.4861111111111111</v>
       </c>
       <c r="E97" t="s">
         <v>7</v>
@@ -5165,11 +5181,11 @@
       <c r="B98" s="1">
         <v>44521</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="2">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="D98" t="s">
         <v>7</v>
-      </c>
-      <c r="D98" s="2">
-        <v>0.51388888888888895</v>
       </c>
       <c r="E98" t="s">
         <v>17</v>
@@ -5194,11 +5210,11 @@
       <c r="B99" s="1">
         <v>44521</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="2">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="D99" t="s">
         <v>7</v>
-      </c>
-      <c r="D99" s="2">
-        <v>0.52777777777777779</v>
       </c>
       <c r="E99" t="s">
         <v>12</v>
@@ -5223,11 +5239,11 @@
       <c r="B100" s="1">
         <v>44527</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="2">
+        <v>0.40625</v>
+      </c>
+      <c r="D100" t="s">
         <v>118</v>
-      </c>
-      <c r="D100" s="2">
-        <v>0.40625</v>
       </c>
       <c r="E100" t="s">
         <v>34</v>
@@ -5250,11 +5266,11 @@
       <c r="B101" s="1">
         <v>44527</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="2">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D101" t="s">
         <v>27</v>
-      </c>
-      <c r="D101" s="2">
-        <v>0.63541666666666663</v>
       </c>
       <c r="E101" t="s">
         <v>119</v>
@@ -5283,11 +5299,11 @@
       <c r="B102" s="1">
         <v>44527</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="2">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="D102" t="s">
         <v>30</v>
-      </c>
-      <c r="D102" s="2">
-        <v>0.67361111111111116</v>
       </c>
       <c r="E102" t="s">
         <v>120</v>
@@ -5316,11 +5332,11 @@
       <c r="B103" s="1">
         <v>44527</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="2">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="D103" t="s">
         <v>44</v>
-      </c>
-      <c r="D103" s="2">
-        <v>0.70486111111111116</v>
       </c>
       <c r="E103" t="s">
         <v>43</v>
@@ -5349,11 +5365,11 @@
       <c r="B104" s="1">
         <v>44527</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="2">
+        <v>0.74652777777777779</v>
+      </c>
+      <c r="D104" t="s">
         <v>40</v>
-      </c>
-      <c r="D104" s="2">
-        <v>0.74652777777777779</v>
       </c>
       <c r="E104" t="s">
         <v>39</v>
@@ -5380,11 +5396,11 @@
       <c r="B105" s="30">
         <v>44527</v>
       </c>
-      <c r="C105" s="8" t="s">
+      <c r="C105" s="20">
+        <v>0.75</v>
+      </c>
+      <c r="D105" s="8" t="s">
         <v>121</v>
-      </c>
-      <c r="D105" s="20">
-        <v>0.75</v>
       </c>
       <c r="E105" s="8" t="s">
         <v>36</v>
@@ -5400,6 +5416,7 @@
       </c>
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
+      <c r="M105" s="8"/>
       <c r="N105" s="20"/>
     </row>
     <row r="106" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5409,11 +5426,11 @@
       <c r="B106" s="1">
         <v>44527</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="2">
+        <v>0.78125</v>
+      </c>
+      <c r="D106" t="s">
         <v>123</v>
-      </c>
-      <c r="D106" s="2">
-        <v>0.78125</v>
       </c>
       <c r="E106" t="s">
         <v>46</v>
@@ -5436,11 +5453,11 @@
       <c r="B107" s="1">
         <v>44534</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D107" t="s">
         <v>124</v>
-      </c>
-      <c r="D107" s="2">
-        <v>0.375</v>
       </c>
       <c r="E107" t="s">
         <v>27</v>
@@ -5463,11 +5480,11 @@
       <c r="B108" s="1">
         <v>44534</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="2">
+        <v>0.40625</v>
+      </c>
+      <c r="D108" t="s">
         <v>125</v>
-      </c>
-      <c r="D108" s="2">
-        <v>0.40625</v>
       </c>
       <c r="E108" t="s">
         <v>30</v>
@@ -5490,11 +5507,11 @@
       <c r="B109" s="1">
         <v>44534</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D109" t="s">
         <v>34</v>
-      </c>
-      <c r="D109" s="2">
-        <v>0.75</v>
       </c>
       <c r="E109" t="s">
         <v>126</v>
@@ -5523,11 +5540,11 @@
       <c r="B110" s="1">
         <v>44534</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="2">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D110" t="s">
         <v>46</v>
-      </c>
-      <c r="D110" s="2">
-        <v>0.82291666666666663</v>
       </c>
       <c r="E110" t="s">
         <v>127</v>
@@ -5554,11 +5571,11 @@
       <c r="B111" s="1">
         <v>44538</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="D111" t="s">
         <v>48</v>
-      </c>
-      <c r="D111" s="2">
-        <v>0.875</v>
       </c>
       <c r="E111" t="s">
         <v>128</v>
@@ -5585,11 +5602,11 @@
       <c r="B112" s="1">
         <v>44541</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D112" t="s">
         <v>129</v>
-      </c>
-      <c r="D112" s="2">
-        <v>0.375</v>
       </c>
       <c r="E112" t="s">
         <v>27</v>
@@ -5612,11 +5629,11 @@
       <c r="B113" s="1">
         <v>44541</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="2">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="D113" t="s">
         <v>56</v>
-      </c>
-      <c r="D113" s="2">
-        <v>0.4548611111111111</v>
       </c>
       <c r="E113" t="s">
         <v>44</v>
@@ -5639,11 +5656,11 @@
       <c r="B114" s="1">
         <v>44541</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D114" t="s">
         <v>130</v>
-      </c>
-      <c r="D114" s="2">
-        <v>0.52083333333333337</v>
       </c>
       <c r="E114" t="s">
         <v>34</v>
@@ -5666,11 +5683,11 @@
       <c r="B115" s="1">
         <v>44541</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" s="2">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D115" t="s">
         <v>131</v>
-      </c>
-      <c r="D115" s="2">
-        <v>0.69791666666666663</v>
       </c>
       <c r="E115" t="s">
         <v>36</v>
@@ -5693,11 +5710,11 @@
       <c r="B116" s="1">
         <v>44541</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="2">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="D116" t="s">
         <v>132</v>
-      </c>
-      <c r="D116" s="2">
-        <v>0.84722222222222221</v>
       </c>
       <c r="E116" t="s">
         <v>46</v>
@@ -5722,11 +5739,11 @@
       <c r="B117" s="1">
         <v>44542</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C117" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D117" t="s">
         <v>58</v>
-      </c>
-      <c r="D117" s="2">
-        <v>0.5</v>
       </c>
       <c r="E117" t="s">
         <v>40</v>
@@ -5749,11 +5766,11 @@
       <c r="B118" s="1">
         <v>44545</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C118" s="2">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D118" t="s">
         <v>133</v>
-      </c>
-      <c r="D118" s="2">
-        <v>0.85416666666666663</v>
       </c>
       <c r="E118" t="s">
         <v>48</v>
@@ -5776,11 +5793,11 @@
       <c r="B119" s="1">
         <v>44548</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" s="2">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D119" t="s">
         <v>27</v>
-      </c>
-      <c r="D119" s="2">
-        <v>0.63888888888888895</v>
       </c>
       <c r="E119" t="s">
         <v>136</v>
@@ -5809,11 +5826,11 @@
       <c r="B120" s="1">
         <v>44548</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" s="2">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D120" t="s">
         <v>30</v>
-      </c>
-      <c r="D120" s="2">
-        <v>0.67708333333333337</v>
       </c>
       <c r="E120" t="s">
         <v>137</v>
@@ -5842,11 +5859,11 @@
       <c r="B121" s="1">
         <v>44548</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D121" t="s">
         <v>34</v>
-      </c>
-      <c r="D121" s="2">
-        <v>0.70833333333333337</v>
       </c>
       <c r="E121" t="s">
         <v>138</v>
@@ -5875,11 +5892,11 @@
       <c r="B122" s="1">
         <v>44548</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C122" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D122" t="s">
         <v>36</v>
-      </c>
-      <c r="D122" s="2">
-        <v>0.75</v>
       </c>
       <c r="E122" t="s">
         <v>139</v>
@@ -5908,11 +5925,11 @@
       <c r="B123" s="1">
         <v>44548</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C123" s="2">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D123" t="s">
         <v>46</v>
-      </c>
-      <c r="D123" s="2">
-        <v>0.82291666666666663</v>
       </c>
       <c r="E123" t="s">
         <v>140</v>
@@ -5939,11 +5956,11 @@
       <c r="B124" s="1">
         <v>44549</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C124" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D124" t="s">
         <v>7</v>
-      </c>
-      <c r="D124" s="2">
-        <v>0.375</v>
       </c>
       <c r="E124" t="s">
         <v>17</v>
@@ -5963,7 +5980,6 @@
         <v>310</v>
       </c>
       <c r="L124" s="1"/>
-      <c r="M124" s="2"/>
       <c r="N124" s="2"/>
     </row>
     <row r="125" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5973,11 +5989,11 @@
       <c r="B125" s="1">
         <v>44549</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C125" s="2">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D125" t="s">
         <v>7</v>
-      </c>
-      <c r="D125" s="2">
-        <v>0.40277777777777773</v>
       </c>
       <c r="E125" t="s">
         <v>20</v>
@@ -5995,7 +6011,6 @@
       </c>
       <c r="K125"/>
       <c r="L125" s="1"/>
-      <c r="M125" s="2"/>
       <c r="N125" s="2"/>
     </row>
     <row r="126" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6005,11 +6020,11 @@
       <c r="B126" s="1">
         <v>44549</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C126" s="2">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D126" t="s">
         <v>21</v>
-      </c>
-      <c r="D126" s="2">
-        <v>0.43055555555555558</v>
       </c>
       <c r="E126" t="s">
         <v>7</v>
@@ -6027,7 +6042,6 @@
       </c>
       <c r="K126"/>
       <c r="L126" s="1"/>
-      <c r="M126" s="2"/>
       <c r="N126" s="2"/>
     </row>
     <row r="127" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6037,11 +6051,11 @@
       <c r="B127" s="1">
         <v>44549</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C127" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D127" t="s">
         <v>22</v>
-      </c>
-      <c r="D127" s="2">
-        <v>0.45833333333333331</v>
       </c>
       <c r="E127" t="s">
         <v>14</v>
@@ -6059,7 +6073,6 @@
       </c>
       <c r="K127"/>
       <c r="L127" s="1"/>
-      <c r="M127" s="2"/>
       <c r="N127" s="2"/>
     </row>
     <row r="128" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6069,11 +6082,11 @@
       <c r="B128" s="1">
         <v>44549</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="2">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="D128" t="s">
         <v>14</v>
-      </c>
-      <c r="D128" s="2">
-        <v>0.4861111111111111</v>
       </c>
       <c r="E128" t="s">
         <v>16</v>
@@ -6091,7 +6104,6 @@
       </c>
       <c r="K128"/>
       <c r="L128" s="1"/>
-      <c r="M128" s="2"/>
       <c r="N128" s="2"/>
     </row>
     <row r="129" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6101,11 +6113,11 @@
       <c r="B129" s="1">
         <v>44549</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C129" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D129" t="s">
         <v>13</v>
-      </c>
-      <c r="D129" s="2">
-        <v>0.5</v>
       </c>
       <c r="E129" t="s">
         <v>14</v>
@@ -6123,7 +6135,6 @@
       </c>
       <c r="K129"/>
       <c r="L129" s="1"/>
-      <c r="M129" s="2"/>
       <c r="N129" s="2"/>
     </row>
     <row r="130" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6133,11 +6144,11 @@
       <c r="B130" s="1">
         <v>44549</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C130" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D130" t="s">
         <v>70</v>
-      </c>
-      <c r="D130" s="2">
-        <v>0.5</v>
       </c>
       <c r="E130" t="s">
         <v>40</v>
@@ -6160,11 +6171,11 @@
       <c r="B131" s="1">
         <v>44569</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C131" s="2">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="D131" t="s">
         <v>27</v>
-      </c>
-      <c r="D131" s="2">
-        <v>0.55555555555555558</v>
       </c>
       <c r="E131" t="s">
         <v>26</v>
@@ -6193,11 +6204,11 @@
       <c r="B132" s="1">
         <v>44569</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C132" s="2">
+        <v>0.59375</v>
+      </c>
+      <c r="D132" t="s">
         <v>30</v>
-      </c>
-      <c r="D132" s="2">
-        <v>0.59375</v>
       </c>
       <c r="E132" t="s">
         <v>29</v>
@@ -6226,11 +6237,11 @@
       <c r="B133" s="1">
         <v>44569</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C133" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D133" t="s">
         <v>34</v>
-      </c>
-      <c r="D133" s="2">
-        <v>0.625</v>
       </c>
       <c r="E133" t="s">
         <v>33</v>
@@ -6259,11 +6270,11 @@
       <c r="B134" s="1">
         <v>44569</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C134" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D134" t="s">
         <v>44</v>
-      </c>
-      <c r="D134" s="2">
-        <v>0.66666666666666663</v>
       </c>
       <c r="E134" t="s">
         <v>80</v>
@@ -6292,11 +6303,11 @@
       <c r="B135" s="1">
         <v>44569</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C135" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D135" t="s">
         <v>36</v>
-      </c>
-      <c r="D135" s="2">
-        <v>0.70833333333333337</v>
       </c>
       <c r="E135" t="s">
         <v>35</v>
@@ -6325,11 +6336,11 @@
       <c r="B136" s="1">
         <v>44569</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C136" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D136" t="s">
         <v>40</v>
-      </c>
-      <c r="D136" s="2">
-        <v>0.75</v>
       </c>
       <c r="E136" t="s">
         <v>87</v>
@@ -6356,11 +6367,11 @@
       <c r="B137" s="1">
         <v>44569</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C137" s="2">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D137" t="s">
         <v>46</v>
-      </c>
-      <c r="D137" s="2">
-        <v>0.82291666666666663</v>
       </c>
       <c r="E137" t="s">
         <v>45</v>
@@ -6387,11 +6398,11 @@
       <c r="B138" s="1">
         <v>44573</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C138" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="D138" t="s">
         <v>48</v>
-      </c>
-      <c r="D138" s="2">
-        <v>0.875</v>
       </c>
       <c r="E138" t="s">
         <v>141</v>
@@ -6420,11 +6431,11 @@
       <c r="B139" s="1">
         <v>44576</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C139" s="2">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D139" t="s">
         <v>14</v>
-      </c>
-      <c r="D139" s="2">
-        <v>0.38541666666666669</v>
       </c>
       <c r="E139" t="s">
         <v>13</v>
@@ -6449,11 +6460,11 @@
       <c r="B140" s="1">
         <v>44576</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C140" s="2">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="D140" t="s">
         <v>22</v>
-      </c>
-      <c r="D140" s="2">
-        <v>0.39930555555555558</v>
       </c>
       <c r="E140" t="s">
         <v>14</v>
@@ -6478,11 +6489,11 @@
       <c r="B141" s="1">
         <v>44576</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C141" s="2">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D141" t="s">
         <v>25</v>
-      </c>
-      <c r="D141" s="2">
-        <v>0.42708333333333331</v>
       </c>
       <c r="E141" t="s">
         <v>14</v>
@@ -6507,11 +6518,11 @@
       <c r="B142" s="1">
         <v>44576</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C142" s="2">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="D142" t="s">
         <v>16</v>
-      </c>
-      <c r="D142" s="2">
-        <v>0.4548611111111111</v>
       </c>
       <c r="E142" t="s">
         <v>14</v>
@@ -6536,11 +6547,11 @@
       <c r="B143" s="1">
         <v>44576</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C143" s="2">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="D143" t="s">
         <v>7</v>
-      </c>
-      <c r="D143" s="2">
-        <v>0.56597222222222221</v>
       </c>
       <c r="E143" t="s">
         <v>17</v>
@@ -6565,11 +6576,11 @@
       <c r="B144" s="1">
         <v>44576</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C144" s="2">
+        <v>0.57986111111111105</v>
+      </c>
+      <c r="D144" t="s">
         <v>20</v>
-      </c>
-      <c r="D144" s="2">
-        <v>0.57986111111111105</v>
       </c>
       <c r="E144" t="s">
         <v>7</v>
@@ -6594,11 +6605,11 @@
       <c r="B145" s="1">
         <v>44576</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C145" s="2">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="D145" t="s">
         <v>7</v>
-      </c>
-      <c r="D145" s="2">
-        <v>0.60763888888888895</v>
       </c>
       <c r="E145" t="s">
         <v>21</v>
@@ -6623,11 +6634,11 @@
       <c r="B146" s="1">
         <v>44576</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C146" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D146" t="s">
         <v>54</v>
-      </c>
-      <c r="D146" s="2">
-        <v>0.58333333333333337</v>
       </c>
       <c r="E146" t="s">
         <v>30</v>
@@ -6650,11 +6661,11 @@
       <c r="B147" s="1">
         <v>44576</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C147" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D147" t="s">
         <v>55</v>
-      </c>
-      <c r="D147" s="2">
-        <v>0.625</v>
       </c>
       <c r="E147" t="s">
         <v>34</v>
@@ -6677,11 +6688,11 @@
       <c r="B148" s="1">
         <v>44576</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C148" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D148" t="s">
         <v>95</v>
-      </c>
-      <c r="D148" s="2">
-        <v>0.70833333333333337</v>
       </c>
       <c r="E148" t="s">
         <v>44</v>
@@ -6704,11 +6715,11 @@
       <c r="B149" s="1">
         <v>44576</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C149" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D149" t="s">
         <v>96</v>
-      </c>
-      <c r="D149" s="2">
-        <v>0.75</v>
       </c>
       <c r="E149" t="s">
         <v>40</v>
@@ -6731,11 +6742,11 @@
       <c r="B150" s="1">
         <v>44576</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C150" s="2">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="D150" t="s">
         <v>59</v>
-      </c>
-      <c r="D150" s="2">
-        <v>0.80208333333333337</v>
       </c>
       <c r="E150" t="s">
         <v>46</v>
@@ -6758,11 +6769,11 @@
       <c r="B151" s="1">
         <v>44577</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C151" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D151" t="s">
         <v>53</v>
-      </c>
-      <c r="D151" s="2">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E151" t="s">
         <v>27</v>
@@ -6785,11 +6796,11 @@
       <c r="B152" s="1">
         <v>44577</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C152" s="2">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="D152" t="s">
         <v>57</v>
-      </c>
-      <c r="D152" s="2">
-        <v>0.60069444444444442</v>
       </c>
       <c r="E152" t="s">
         <v>36</v>
@@ -6812,11 +6823,11 @@
       <c r="B153" s="1">
         <v>44583</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C153" s="2">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="D153" t="s">
         <v>27</v>
-      </c>
-      <c r="D153" s="2">
-        <v>0.55555555555555558</v>
       </c>
       <c r="E153" t="s">
         <v>61</v>
@@ -6845,11 +6856,11 @@
       <c r="B154" s="1">
         <v>44583</v>
       </c>
-      <c r="C154" t="s">
+      <c r="C154" s="2">
+        <v>0.59375</v>
+      </c>
+      <c r="D154" t="s">
         <v>30</v>
-      </c>
-      <c r="D154" s="2">
-        <v>0.59375</v>
       </c>
       <c r="E154" t="s">
         <v>64</v>
@@ -6878,11 +6889,11 @@
       <c r="B155" s="1">
         <v>44583</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C155" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D155" t="s">
         <v>34</v>
-      </c>
-      <c r="D155" s="2">
-        <v>0.625</v>
       </c>
       <c r="E155" t="s">
         <v>71</v>
@@ -6911,11 +6922,11 @@
       <c r="B156" s="1">
         <v>44583</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C156" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D156" t="s">
         <v>44</v>
-      </c>
-      <c r="D156" s="2">
-        <v>0.66666666666666663</v>
       </c>
       <c r="E156" t="s">
         <v>106</v>
@@ -6947,11 +6958,11 @@
       <c r="B157" s="1">
         <v>44583</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C157" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D157" t="s">
         <v>36</v>
-      </c>
-      <c r="D157" s="2">
-        <v>0.70833333333333337</v>
       </c>
       <c r="E157" t="s">
         <v>295</v>
@@ -6983,11 +6994,11 @@
       <c r="B158" s="1">
         <v>44583</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C158" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D158" t="s">
         <v>40</v>
-      </c>
-      <c r="D158" s="2">
-        <v>0.75</v>
       </c>
       <c r="E158" t="s">
         <v>103</v>
@@ -7014,11 +7025,11 @@
       <c r="B159" s="1">
         <v>44584</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C159" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D159" t="s">
         <v>74</v>
-      </c>
-      <c r="D159" s="2">
-        <v>0.45833333333333331</v>
       </c>
       <c r="E159" t="s">
         <v>46</v>
@@ -7041,11 +7052,11 @@
       <c r="B160" s="1">
         <v>44587</v>
       </c>
-      <c r="C160" t="s">
+      <c r="C160" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="D160" t="s">
         <v>48</v>
-      </c>
-      <c r="D160" s="2">
-        <v>0.875</v>
       </c>
       <c r="E160" t="s">
         <v>47</v>
@@ -7074,11 +7085,11 @@
       <c r="B161" s="1">
         <v>44590</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C161" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D161" t="s">
         <v>84</v>
-      </c>
-      <c r="D161" s="2">
-        <v>0.375</v>
       </c>
       <c r="E161" t="s">
         <v>30</v>
@@ -7101,11 +7112,11 @@
       <c r="B162" s="1">
         <v>44590</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C162" s="2">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D162" t="s">
         <v>7</v>
-      </c>
-      <c r="D162" s="2">
-        <v>0.3888888888888889</v>
       </c>
       <c r="E162" t="s">
         <v>11</v>
@@ -7130,11 +7141,11 @@
       <c r="B163" s="1">
         <v>44590</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C163" s="2">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D163" t="s">
         <v>7</v>
-      </c>
-      <c r="D163" s="2">
-        <v>0.40277777777777773</v>
       </c>
       <c r="E163" t="s">
         <v>12</v>
@@ -7159,11 +7170,11 @@
       <c r="B164" s="1">
         <v>44590</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C164" s="2">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D164" t="s">
         <v>7</v>
-      </c>
-      <c r="D164" s="2">
-        <v>0.43055555555555558</v>
       </c>
       <c r="E164" t="s">
         <v>8</v>
@@ -7188,11 +7199,11 @@
       <c r="B165" s="1">
         <v>44590</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C165" s="2">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D165" t="s">
         <v>15</v>
-      </c>
-      <c r="D165" s="2">
-        <v>0.3888888888888889</v>
       </c>
       <c r="E165" t="s">
         <v>14</v>
@@ -7217,11 +7228,11 @@
       <c r="B166" s="1">
         <v>44590</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C166" s="2">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D166" t="s">
         <v>14</v>
-      </c>
-      <c r="D166" s="2">
-        <v>0.43055555555555558</v>
       </c>
       <c r="E166" t="s">
         <v>25</v>
@@ -7246,11 +7257,11 @@
       <c r="B167" s="1">
         <v>44590</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C167" s="2">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D167" t="s">
         <v>14</v>
-      </c>
-      <c r="D167" s="2">
-        <v>0.44444444444444442</v>
       </c>
       <c r="E167" t="s">
         <v>307</v>
@@ -7275,11 +7286,11 @@
       <c r="B168" s="1">
         <v>44590</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C168" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D168" t="s">
         <v>83</v>
-      </c>
-      <c r="D168" s="2">
-        <v>0.39583333333333331</v>
       </c>
       <c r="E168" t="s">
         <v>27</v>
@@ -7302,11 +7313,11 @@
       <c r="B169" s="1">
         <v>44590</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C169" s="2">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D169" t="s">
         <v>112</v>
-      </c>
-      <c r="D169" s="2">
-        <v>0.44444444444444442</v>
       </c>
       <c r="E169" t="s">
         <v>44</v>
@@ -7329,11 +7340,11 @@
       <c r="B170" s="1">
         <v>44590</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C170" s="2">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D170" t="s">
         <v>15</v>
-      </c>
-      <c r="D170" s="2">
-        <v>0.44444444444444442</v>
       </c>
       <c r="E170" t="s">
         <v>14</v>
@@ -7356,11 +7367,11 @@
       <c r="B171" s="1">
         <v>44590</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C171" s="2">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D171" t="s">
         <v>46</v>
-      </c>
-      <c r="D171" s="2">
-        <v>0.82291666666666663</v>
       </c>
       <c r="E171" t="s">
         <v>88</v>
@@ -7387,11 +7398,11 @@
       <c r="B172" s="1">
         <v>44591</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C172" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D172" t="s">
         <v>114</v>
-      </c>
-      <c r="D172" s="2">
-        <v>0.45833333333333331</v>
       </c>
       <c r="E172" t="s">
         <v>40</v>
@@ -7414,11 +7425,11 @@
       <c r="B173" s="1">
         <v>44591</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C173" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D173" t="s">
         <v>86</v>
-      </c>
-      <c r="D173" s="2">
-        <v>0.45833333333333331</v>
       </c>
       <c r="E173" t="s">
         <v>36</v>
@@ -7441,11 +7452,11 @@
       <c r="B174" s="1">
         <v>44591</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C174" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D174" t="s">
         <v>85</v>
-      </c>
-      <c r="D174" s="2">
-        <v>0.45833333333333331</v>
       </c>
       <c r="E174" t="s">
         <v>34</v>
@@ -7468,11 +7479,11 @@
       <c r="B175" s="1">
         <v>44594</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C175" s="2">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="D175" t="s">
         <v>60</v>
-      </c>
-      <c r="D175" s="2">
-        <v>0.86458333333333337</v>
       </c>
       <c r="E175" t="s">
         <v>48</v>
@@ -7495,11 +7506,11 @@
       <c r="B176" s="9">
         <v>44597</v>
       </c>
-      <c r="C176" s="8" t="s">
+      <c r="C176" s="10">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="D176" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="D176" s="10">
-        <v>0.62847222222222221</v>
       </c>
       <c r="E176" s="8" t="s">
         <v>92</v>
@@ -7519,6 +7530,7 @@
       <c r="J176" s="14" t="s">
         <v>260</v>
       </c>
+      <c r="M176" s="8"/>
       <c r="N176" s="10"/>
     </row>
     <row r="177" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7528,11 +7540,11 @@
       <c r="B177" s="1">
         <v>44597</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C177" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D177" t="s">
         <v>34</v>
-      </c>
-      <c r="D177" s="2">
-        <v>0.66666666666666663</v>
       </c>
       <c r="E177" t="s">
         <v>91</v>
@@ -7561,11 +7573,11 @@
       <c r="B178" s="1">
         <v>44597</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C178" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D178" t="s">
         <v>36</v>
-      </c>
-      <c r="D178" s="2">
-        <v>0.70833333333333337</v>
       </c>
       <c r="E178" t="s">
         <v>98</v>
@@ -7594,11 +7606,11 @@
       <c r="B179" s="1">
         <v>44597</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C179" s="2">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="D179" t="s">
         <v>97</v>
-      </c>
-      <c r="D179" s="2">
-        <v>0.86111111111111116</v>
       </c>
       <c r="E179" t="s">
         <v>46</v>
@@ -7621,11 +7633,11 @@
       <c r="B180" s="1">
         <v>44598</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C180" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D180" t="s">
         <v>39</v>
-      </c>
-      <c r="D180" s="2">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E180" t="s">
         <v>40</v>
@@ -7648,11 +7660,11 @@
       <c r="B181" s="1">
         <v>44598</v>
       </c>
-      <c r="C181" t="s">
+      <c r="C181" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D181" t="s">
         <v>43</v>
-      </c>
-      <c r="D181" s="2">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E181" t="s">
         <v>44</v>
@@ -7675,11 +7687,11 @@
       <c r="B182" s="1">
         <v>44604</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C182" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D182" t="s">
         <v>7</v>
-      </c>
-      <c r="D182" s="2">
-        <v>0.375</v>
       </c>
       <c r="E182" t="s">
         <v>8</v>
@@ -7704,11 +7716,11 @@
       <c r="B183" s="1">
         <v>44604</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C183" s="2">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D183" t="s">
         <v>11</v>
-      </c>
-      <c r="D183" s="2">
-        <v>0.40277777777777773</v>
       </c>
       <c r="E183" t="s">
         <v>7</v>
@@ -7733,11 +7745,11 @@
       <c r="B184" s="1">
         <v>44604</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C184" s="2">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D184" t="s">
         <v>7</v>
-      </c>
-      <c r="D184" s="2">
-        <v>0.44444444444444442</v>
       </c>
       <c r="E184" t="s">
         <v>12</v>
@@ -7762,11 +7774,11 @@
       <c r="B185" s="1">
         <v>44604</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C185" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D185" t="s">
         <v>14</v>
-      </c>
-      <c r="D185" s="2">
-        <v>0.4375</v>
       </c>
       <c r="E185" t="s">
         <v>15</v>
@@ -7791,11 +7803,11 @@
       <c r="B186" s="1">
         <v>44604</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C186" s="2">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="D186" t="s">
         <v>307</v>
-      </c>
-      <c r="D186" s="2">
-        <v>0.46527777777777773</v>
       </c>
       <c r="E186" t="s">
         <v>14</v>
@@ -7820,11 +7832,11 @@
       <c r="B187" s="1">
         <v>44604</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C187" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D187" t="s">
         <v>25</v>
-      </c>
-      <c r="D187" s="2">
-        <v>0.47916666666666669</v>
       </c>
       <c r="E187" t="s">
         <v>14</v>
@@ -7849,11 +7861,11 @@
       <c r="B188" s="1">
         <v>44604</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C188" s="2">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="D188" t="s">
         <v>99</v>
-      </c>
-      <c r="D188" s="2">
-        <v>0.41319444444444442</v>
       </c>
       <c r="E188" t="s">
         <v>27</v>
@@ -7876,11 +7888,11 @@
       <c r="B189" s="1">
         <v>44604</v>
       </c>
-      <c r="C189" t="s">
+      <c r="C189" s="2">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="D189" t="s">
         <v>100</v>
-      </c>
-      <c r="D189" s="2">
-        <v>0.4513888888888889</v>
       </c>
       <c r="E189" t="s">
         <v>30</v>
@@ -7903,11 +7915,11 @@
       <c r="B190" s="1">
         <v>44604</v>
       </c>
-      <c r="C190" t="s">
+      <c r="C190" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D190" t="s">
         <v>101</v>
-      </c>
-      <c r="D190" s="2">
-        <v>0.45833333333333331</v>
       </c>
       <c r="E190" t="s">
         <v>34</v>
@@ -7930,11 +7942,11 @@
       <c r="B191" s="1">
         <v>44604</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C191" s="2">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="D191" t="s">
         <v>102</v>
-      </c>
-      <c r="D191" s="2">
-        <v>0.47569444444444442</v>
       </c>
       <c r="E191" t="s">
         <v>36</v>
@@ -7957,11 +7969,11 @@
       <c r="B192" s="1">
         <v>44604</v>
       </c>
-      <c r="C192" t="s">
+      <c r="C192" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D192" t="s">
         <v>44</v>
-      </c>
-      <c r="D192" s="2">
-        <v>0.70833333333333337</v>
       </c>
       <c r="E192" t="s">
         <v>56</v>
@@ -7990,11 +8002,11 @@
       <c r="B193" s="1">
         <v>44604</v>
       </c>
-      <c r="C193" t="s">
+      <c r="C193" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D193" t="s">
         <v>40</v>
-      </c>
-      <c r="D193" s="2">
-        <v>0.75</v>
       </c>
       <c r="E193" t="s">
         <v>58</v>
@@ -8021,11 +8033,11 @@
       <c r="B194" s="1">
         <v>44604</v>
       </c>
-      <c r="C194" t="s">
+      <c r="C194" s="2">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D194" t="s">
         <v>46</v>
-      </c>
-      <c r="D194" s="2">
-        <v>0.82291666666666663</v>
       </c>
       <c r="E194" t="s">
         <v>107</v>
@@ -8052,11 +8064,11 @@
       <c r="B195" s="1">
         <v>44608</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C195" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="D195" t="s">
         <v>48</v>
-      </c>
-      <c r="D195" s="2">
-        <v>0.875</v>
       </c>
       <c r="E195" t="s">
         <v>75</v>
@@ -8085,11 +8097,11 @@
       <c r="B196" s="4">
         <v>44625</v>
       </c>
-      <c r="C196" s="3" t="s">
+      <c r="C196" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D196" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D196" s="5">
-        <v>0.375</v>
       </c>
       <c r="E196" s="3" t="s">
         <v>8</v>
@@ -8109,6 +8121,7 @@
       <c r="J196" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M196" s="3"/>
       <c r="N196" s="5"/>
     </row>
     <row r="197" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8118,11 +8131,11 @@
       <c r="B197" s="4">
         <v>44625</v>
       </c>
-      <c r="C197" s="3" t="s">
+      <c r="C197" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D197" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="D197" s="5">
-        <v>0.375</v>
       </c>
       <c r="E197" s="3" t="s">
         <v>20</v>
@@ -8142,6 +8155,7 @@
       <c r="J197" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M197" s="3"/>
       <c r="N197" s="5"/>
     </row>
     <row r="198" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8151,11 +8165,11 @@
       <c r="B198" s="4">
         <v>44625</v>
       </c>
-      <c r="C198" s="3" t="s">
+      <c r="C198" s="5">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D198" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="D198" s="5">
-        <v>0.3888888888888889</v>
       </c>
       <c r="E198" s="3" t="s">
         <v>12</v>
@@ -8175,6 +8189,7 @@
       <c r="J198" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M198" s="3"/>
       <c r="N198" s="5"/>
     </row>
     <row r="199" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8184,11 +8199,11 @@
       <c r="B199" s="4">
         <v>44625</v>
       </c>
-      <c r="C199" s="3" t="s">
+      <c r="C199" s="5">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D199" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D199" s="5">
-        <v>0.3888888888888889</v>
       </c>
       <c r="E199" s="3" t="s">
         <v>17</v>
@@ -8208,6 +8223,7 @@
       <c r="J199" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M199" s="3"/>
       <c r="N199" s="5"/>
     </row>
     <row r="200" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8217,11 +8233,11 @@
       <c r="B200" s="4">
         <v>44625</v>
       </c>
-      <c r="C200" s="3" t="s">
+      <c r="C200" s="5">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D200" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="D200" s="5">
-        <v>0.40277777777777773</v>
       </c>
       <c r="E200" s="3" t="s">
         <v>8</v>
@@ -8241,6 +8257,7 @@
       <c r="J200" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M200" s="3"/>
       <c r="N200" s="5"/>
     </row>
     <row r="201" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8250,11 +8267,11 @@
       <c r="B201" s="4">
         <v>44625</v>
       </c>
-      <c r="C201" s="3" t="s">
+      <c r="C201" s="5">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D201" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="D201" s="5">
-        <v>0.40277777777777773</v>
       </c>
       <c r="E201" s="3" t="s">
         <v>7</v>
@@ -8274,6 +8291,7 @@
       <c r="J201" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M201" s="3"/>
       <c r="N201" s="5"/>
     </row>
     <row r="202" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8283,11 +8301,11 @@
       <c r="B202" s="4">
         <v>44625</v>
       </c>
-      <c r="C202" s="3" t="s">
+      <c r="C202" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D202" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="D202" s="5">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E202" s="3" t="s">
         <v>11</v>
@@ -8307,6 +8325,7 @@
       <c r="J202" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M202" s="3"/>
       <c r="N202" s="5"/>
     </row>
     <row r="203" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8316,11 +8335,11 @@
       <c r="B203" s="4">
         <v>44625</v>
       </c>
-      <c r="C203" s="3" t="s">
+      <c r="C203" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D203" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="D203" s="5">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E203" s="3" t="s">
         <v>17</v>
@@ -8340,6 +8359,7 @@
       <c r="J203" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M203" s="3"/>
       <c r="N203" s="5"/>
     </row>
     <row r="204" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8349,11 +8369,11 @@
       <c r="B204" s="4">
         <v>44625</v>
       </c>
-      <c r="C204" s="3" t="s">
+      <c r="C204" s="5">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D204" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="D204" s="5">
-        <v>0.43055555555555558</v>
       </c>
       <c r="E204" s="3" t="s">
         <v>12</v>
@@ -8373,6 +8393,7 @@
       <c r="J204" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M204" s="3"/>
       <c r="N204" s="5"/>
     </row>
     <row r="205" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8382,11 +8403,11 @@
       <c r="B205" s="4">
         <v>44625</v>
       </c>
-      <c r="C205" s="3" t="s">
+      <c r="C205" s="5">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D205" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D205" s="5">
-        <v>0.43055555555555558</v>
       </c>
       <c r="E205" s="3" t="s">
         <v>21</v>
@@ -8406,6 +8427,7 @@
       <c r="J205" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M205" s="3"/>
       <c r="N205" s="5"/>
     </row>
     <row r="206" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8415,11 +8437,11 @@
       <c r="B206" s="4">
         <v>44625</v>
       </c>
-      <c r="C206" s="3" t="s">
+      <c r="C206" s="5">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D206" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="D206" s="5">
-        <v>0.44444444444444442</v>
       </c>
       <c r="E206" s="3" t="s">
         <v>17</v>
@@ -8439,6 +8461,7 @@
       <c r="J206" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M206" s="3"/>
       <c r="N206" s="5"/>
     </row>
     <row r="207" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8448,11 +8471,11 @@
       <c r="B207" s="1">
         <v>44625</v>
       </c>
-      <c r="C207" t="s">
+      <c r="C207" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D207" t="s">
         <v>14</v>
-      </c>
-      <c r="D207" s="2">
-        <v>0.375</v>
       </c>
       <c r="E207" t="s">
         <v>13</v>
@@ -8477,11 +8500,11 @@
       <c r="B208" s="1">
         <v>44625</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C208" s="2">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D208" t="s">
         <v>22</v>
-      </c>
-      <c r="D208" s="2">
-        <v>0.3888888888888889</v>
       </c>
       <c r="E208" t="s">
         <v>14</v>
@@ -8506,11 +8529,11 @@
       <c r="B209" s="1">
         <v>44625</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C209" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D209" t="s">
         <v>25</v>
-      </c>
-      <c r="D209" s="2">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E209" t="s">
         <v>14</v>
@@ -8535,11 +8558,11 @@
       <c r="B210" s="1">
         <v>44625</v>
       </c>
-      <c r="C210" t="s">
+      <c r="C210" s="2">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D210" t="s">
         <v>16</v>
-      </c>
-      <c r="D210" s="2">
-        <v>0.44444444444444442</v>
       </c>
       <c r="E210" t="s">
         <v>14</v>
@@ -8564,11 +8587,11 @@
       <c r="B211" s="1">
         <v>44625</v>
       </c>
-      <c r="C211" t="s">
+      <c r="C211" s="2">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="D211" t="s">
         <v>286</v>
-      </c>
-      <c r="D211" s="2">
-        <v>0.46527777777777773</v>
       </c>
       <c r="E211" t="s">
         <v>34</v>
@@ -8594,11 +8617,11 @@
       <c r="B212" s="1">
         <v>44625</v>
       </c>
-      <c r="C212" t="s">
+      <c r="C212" s="2">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D212" t="s">
         <v>27</v>
-      </c>
-      <c r="D212" s="2">
-        <v>0.63888888888888895</v>
       </c>
       <c r="E212" t="s">
         <v>109</v>
@@ -8627,11 +8650,11 @@
       <c r="B213" s="1">
         <v>44625</v>
       </c>
-      <c r="C213" t="s">
+      <c r="C213" s="2">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D213" t="s">
         <v>30</v>
-      </c>
-      <c r="D213" s="2">
-        <v>0.67708333333333337</v>
       </c>
       <c r="E213" t="s">
         <v>108</v>
@@ -8660,11 +8683,11 @@
       <c r="B214" s="1">
         <v>44625</v>
       </c>
-      <c r="C214" t="s">
+      <c r="C214" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D214" t="s">
         <v>44</v>
-      </c>
-      <c r="D214" s="2">
-        <v>0.70833333333333337</v>
       </c>
       <c r="E214" t="s">
         <v>67</v>
@@ -8693,11 +8716,11 @@
       <c r="B215" s="1">
         <v>44625</v>
       </c>
-      <c r="C215" t="s">
+      <c r="C215" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D215" t="s">
         <v>40</v>
-      </c>
-      <c r="D215" s="2">
-        <v>0.75</v>
       </c>
       <c r="E215" t="s">
         <v>70</v>
@@ -8724,11 +8747,11 @@
       <c r="B216" s="1">
         <v>44626</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C216" s="2">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="D216" t="s">
         <v>115</v>
-      </c>
-      <c r="D216" s="2">
-        <v>0.51388888888888895</v>
       </c>
       <c r="E216" t="s">
         <v>46</v>
@@ -8751,11 +8774,11 @@
       <c r="B217" s="1">
         <v>44626</v>
       </c>
-      <c r="C217" t="s">
+      <c r="C217" s="2">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D217" t="s">
         <v>113</v>
-      </c>
-      <c r="D217" s="2">
-        <v>0.55208333333333337</v>
       </c>
       <c r="E217" t="s">
         <v>36</v>
@@ -8778,11 +8801,11 @@
       <c r="B218" s="1">
         <v>44632</v>
       </c>
-      <c r="C218" t="s">
+      <c r="C218" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D218" t="s">
         <v>119</v>
-      </c>
-      <c r="D218" s="2">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E218" t="s">
         <v>27</v>
@@ -8805,11 +8828,11 @@
       <c r="B219" s="1">
         <v>44632</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C219" s="2">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="D219" t="s">
         <v>120</v>
-      </c>
-      <c r="D219" s="2">
-        <v>0.4548611111111111</v>
       </c>
       <c r="E219" t="s">
         <v>30</v>
@@ -8832,11 +8855,11 @@
       <c r="B220" s="1">
         <v>44632</v>
       </c>
-      <c r="C220" t="s">
+      <c r="C220" s="2">
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="D220" t="s">
         <v>80</v>
-      </c>
-      <c r="D220" s="2">
-        <v>0.49652777777777773</v>
       </c>
       <c r="E220" t="s">
         <v>44</v>
@@ -8859,11 +8882,11 @@
       <c r="B221" s="1">
         <v>44632</v>
       </c>
-      <c r="C221" t="s">
+      <c r="C221" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D221" t="s">
         <v>34</v>
-      </c>
-      <c r="D221" s="2">
-        <v>0.70833333333333337</v>
       </c>
       <c r="E221" t="s">
         <v>118</v>
@@ -8892,11 +8915,11 @@
       <c r="B222" s="1">
         <v>44632</v>
       </c>
-      <c r="C222" t="s">
+      <c r="C222" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D222" t="s">
         <v>36</v>
-      </c>
-      <c r="D222" s="2">
-        <v>0.75</v>
       </c>
       <c r="E222" t="s">
         <v>121</v>
@@ -8925,11 +8948,11 @@
       <c r="B223" s="1">
         <v>44632</v>
       </c>
-      <c r="C223" t="s">
+      <c r="C223" s="2">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="D223" t="s">
         <v>87</v>
-      </c>
-      <c r="D223" s="2">
-        <v>0.78472222222222221</v>
       </c>
       <c r="E223" t="s">
         <v>40</v>
@@ -8952,11 +8975,11 @@
       <c r="B224" s="1">
         <v>44632</v>
       </c>
-      <c r="C224" t="s">
+      <c r="C224" s="2">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D224" t="s">
         <v>46</v>
-      </c>
-      <c r="D224" s="2">
-        <v>0.82291666666666663</v>
       </c>
       <c r="E224" t="s">
         <v>123</v>
@@ -8983,11 +9006,11 @@
       <c r="B225" s="1">
         <v>44639</v>
       </c>
-      <c r="C225" t="s">
+      <c r="C225" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D225" t="s">
         <v>15</v>
-      </c>
-      <c r="D225" s="2">
-        <v>0.54166666666666663</v>
       </c>
       <c r="E225" t="s">
         <v>14</v>
@@ -9012,11 +9035,11 @@
       <c r="B226" s="1">
         <v>44639</v>
       </c>
-      <c r="C226" t="s">
+      <c r="C226" s="2">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="D226" t="s">
         <v>14</v>
-      </c>
-      <c r="D226" s="2">
-        <v>0.56944444444444442</v>
       </c>
       <c r="E226" t="s">
         <v>307</v>
@@ -9041,11 +9064,11 @@
       <c r="B227" s="1">
         <v>44639</v>
       </c>
-      <c r="C227" t="s">
+      <c r="C227" s="2">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="D227" t="s">
         <v>14</v>
-      </c>
-      <c r="D227" s="2">
-        <v>0.59722222222222221</v>
       </c>
       <c r="E227" t="s">
         <v>25</v>
@@ -9070,11 +9093,11 @@
       <c r="B228" s="1">
         <v>44639</v>
       </c>
-      <c r="C228" t="s">
+      <c r="C228" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D228" t="s">
         <v>8</v>
-      </c>
-      <c r="D228" s="2">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E228" t="s">
         <v>7</v>
@@ -9099,11 +9122,11 @@
       <c r="B229" s="1">
         <v>44639</v>
       </c>
-      <c r="C229" t="s">
+      <c r="C229" s="2">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D229" t="s">
         <v>7</v>
-      </c>
-      <c r="D229" s="2">
-        <v>0.44444444444444442</v>
       </c>
       <c r="E229" t="s">
         <v>11</v>
@@ -9128,11 +9151,11 @@
       <c r="B230" s="1">
         <v>44639</v>
       </c>
-      <c r="C230" t="s">
+      <c r="C230" s="2">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="D230" t="s">
         <v>12</v>
-      </c>
-      <c r="D230" s="2">
-        <v>0.47222222222222227</v>
       </c>
       <c r="E230" t="s">
         <v>7</v>
@@ -9157,11 +9180,11 @@
       <c r="B231" s="1">
         <v>44639</v>
       </c>
-      <c r="C231" t="s">
+      <c r="C231" s="2">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="D231" t="s">
         <v>126</v>
-      </c>
-      <c r="D231" s="2">
-        <v>0.4826388888888889</v>
       </c>
       <c r="E231" t="s">
         <v>34</v>
@@ -9184,11 +9207,11 @@
       <c r="B232" s="1">
         <v>44639</v>
       </c>
-      <c r="C232" t="s">
+      <c r="C232" s="2">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D232" t="s">
         <v>27</v>
-      </c>
-      <c r="D232" s="2">
-        <v>0.63888888888888895</v>
       </c>
       <c r="E232" t="s">
         <v>124</v>
@@ -9217,11 +9240,11 @@
       <c r="B233" s="1">
         <v>44639</v>
       </c>
-      <c r="C233" t="s">
+      <c r="C233" s="2">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D233" t="s">
         <v>30</v>
-      </c>
-      <c r="D233" s="2">
-        <v>0.67708333333333337</v>
       </c>
       <c r="E233" t="s">
         <v>125</v>
@@ -9250,11 +9273,11 @@
       <c r="B234" s="1">
         <v>44639</v>
       </c>
-      <c r="C234" t="s">
+      <c r="C234" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D234" t="s">
         <v>44</v>
-      </c>
-      <c r="D234" s="2">
-        <v>0.70833333333333337</v>
       </c>
       <c r="E234" t="s">
         <v>95</v>
@@ -9283,11 +9306,11 @@
       <c r="B235" s="1">
         <v>44639</v>
       </c>
-      <c r="C235" t="s">
+      <c r="C235" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D235" t="s">
         <v>40</v>
-      </c>
-      <c r="D235" s="2">
-        <v>0.75</v>
       </c>
       <c r="E235" t="s">
         <v>96</v>
@@ -9314,11 +9337,11 @@
       <c r="B236" s="1">
         <v>44639</v>
       </c>
-      <c r="C236" t="s">
+      <c r="C236" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D236" t="s">
         <v>127</v>
-      </c>
-      <c r="D236" s="2">
-        <v>0.79166666666666663</v>
       </c>
       <c r="E236" t="s">
         <v>46</v>
@@ -9341,11 +9364,11 @@
       <c r="B237" s="9">
         <v>44653</v>
       </c>
-      <c r="C237" s="8" t="s">
+      <c r="C237" s="10">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="D237" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="D237" s="10">
-        <v>0.67013888888888884</v>
       </c>
       <c r="E237" s="8" t="s">
         <v>129</v>
@@ -9365,6 +9388,7 @@
       <c r="J237" s="14" t="s">
         <v>276</v>
       </c>
+      <c r="M237" s="8"/>
       <c r="N237" s="10"/>
     </row>
     <row r="238" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9374,11 +9398,11 @@
       <c r="B238" s="1">
         <v>44653</v>
       </c>
-      <c r="C238" t="s">
+      <c r="C238" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D238" t="s">
         <v>34</v>
-      </c>
-      <c r="D238" s="2">
-        <v>0.70833333333333337</v>
       </c>
       <c r="E238" t="s">
         <v>130</v>
@@ -9407,11 +9431,11 @@
       <c r="B239" s="1">
         <v>44653</v>
       </c>
-      <c r="C239" t="s">
+      <c r="C239" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D239" t="s">
         <v>36</v>
-      </c>
-      <c r="D239" s="2">
-        <v>0.75</v>
       </c>
       <c r="E239" t="s">
         <v>131</v>
@@ -9440,11 +9464,11 @@
       <c r="B240" s="1">
         <v>44653</v>
       </c>
-      <c r="C240" t="s">
+      <c r="C240" s="2">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D240" t="s">
         <v>46</v>
-      </c>
-      <c r="D240" s="2">
-        <v>0.82291666666666663</v>
       </c>
       <c r="E240" t="s">
         <v>132</v>
@@ -9471,11 +9495,11 @@
       <c r="B241" s="1">
         <v>44654</v>
       </c>
-      <c r="C241" t="s">
+      <c r="C241" s="2">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="D241" t="s">
         <v>103</v>
-      </c>
-      <c r="D241" s="2">
-        <v>0.4861111111111111</v>
       </c>
       <c r="E241" t="s">
         <v>40</v>
@@ -9498,11 +9522,11 @@
       <c r="B242" s="1">
         <v>44654</v>
       </c>
-      <c r="C242" t="s">
+      <c r="C242" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D242" t="s">
         <v>106</v>
-      </c>
-      <c r="D242" s="2">
-        <v>0.5</v>
       </c>
       <c r="E242" t="s">
         <v>44</v>
@@ -9525,11 +9549,11 @@
       <c r="B243" s="1">
         <v>44659</v>
       </c>
-      <c r="C243" t="s">
+      <c r="C243" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="D243" t="s">
         <v>128</v>
-      </c>
-      <c r="D243" s="2">
-        <v>0.875</v>
       </c>
       <c r="E243" t="s">
         <v>48</v>
@@ -9552,11 +9576,11 @@
       <c r="B244" s="4">
         <v>44660</v>
       </c>
-      <c r="C244" s="3" t="s">
+      <c r="C244" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D244" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="D244" s="5">
-        <v>0.375</v>
       </c>
       <c r="E244" s="3" t="s">
         <v>14</v>
@@ -9576,6 +9600,7 @@
       <c r="J244" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M244" s="3"/>
       <c r="N244" s="5"/>
     </row>
     <row r="245" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9585,11 +9610,11 @@
       <c r="B245" s="4">
         <v>44660</v>
       </c>
-      <c r="C245" s="3" t="s">
+      <c r="C245" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="D245" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D245" s="5">
-        <v>0.375</v>
       </c>
       <c r="E245" s="3" t="s">
         <v>15</v>
@@ -9609,6 +9634,7 @@
       <c r="J245" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M245" s="3"/>
       <c r="N245" s="5"/>
     </row>
     <row r="246" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9618,11 +9644,11 @@
       <c r="B246" s="4">
         <v>44660</v>
       </c>
-      <c r="C246" s="3" t="s">
+      <c r="C246" s="5">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D246" s="3" t="s">
         <v>307</v>
-      </c>
-      <c r="D246" s="5">
-        <v>0.3888888888888889</v>
       </c>
       <c r="E246" s="3" t="s">
         <v>13</v>
@@ -9642,6 +9668,7 @@
       <c r="J246" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M246" s="3"/>
       <c r="N246" s="5"/>
     </row>
     <row r="247" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9651,11 +9678,11 @@
       <c r="B247" s="4">
         <v>44660</v>
       </c>
-      <c r="C247" s="3" t="s">
+      <c r="C247" s="5">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D247" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="D247" s="5">
-        <v>0.3888888888888889</v>
       </c>
       <c r="E247" s="3" t="s">
         <v>15</v>
@@ -9675,6 +9702,7 @@
       <c r="J247" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M247" s="3"/>
       <c r="N247" s="5"/>
     </row>
     <row r="248" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9684,11 +9712,11 @@
       <c r="B248" s="4">
         <v>44660</v>
       </c>
-      <c r="C248" s="3" t="s">
+      <c r="C248" s="5">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D248" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="D248" s="5">
-        <v>0.40277777777777773</v>
       </c>
       <c r="E248" s="3" t="s">
         <v>25</v>
@@ -9708,6 +9736,7 @@
       <c r="J248" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M248" s="3"/>
       <c r="N248" s="5"/>
     </row>
     <row r="249" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9717,11 +9746,11 @@
       <c r="B249" s="4">
         <v>44660</v>
       </c>
-      <c r="C249" s="3" t="s">
+      <c r="C249" s="5">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D249" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="D249" s="5">
-        <v>0.40277777777777773</v>
       </c>
       <c r="E249" s="3" t="s">
         <v>16</v>
@@ -9741,6 +9770,7 @@
       <c r="J249" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M249" s="3"/>
       <c r="N249" s="5"/>
     </row>
     <row r="250" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9750,11 +9780,11 @@
       <c r="B250" s="4">
         <v>44660</v>
       </c>
-      <c r="C250" s="3" t="s">
+      <c r="C250" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D250" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D250" s="5">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E250" s="3" t="s">
         <v>307</v>
@@ -9774,6 +9804,7 @@
       <c r="J250" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M250" s="3"/>
       <c r="N250" s="5"/>
     </row>
     <row r="251" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9783,11 +9814,11 @@
       <c r="B251" s="4">
         <v>44660</v>
       </c>
-      <c r="C251" s="3" t="s">
+      <c r="C251" s="5">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D251" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D251" s="5">
-        <v>0.41666666666666669</v>
       </c>
       <c r="E251" s="3" t="s">
         <v>14</v>
@@ -9807,6 +9838,7 @@
       <c r="J251" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M251" s="3"/>
       <c r="N251" s="5"/>
     </row>
     <row r="252" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9816,11 +9848,11 @@
       <c r="B252" s="4">
         <v>44660</v>
       </c>
-      <c r="C252" s="3" t="s">
+      <c r="C252" s="5">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D252" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="D252" s="5">
-        <v>0.43055555555555558</v>
       </c>
       <c r="E252" s="3" t="s">
         <v>307</v>
@@ -9840,6 +9872,7 @@
       <c r="J252" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M252" s="3"/>
       <c r="N252" s="5"/>
     </row>
     <row r="253" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9849,11 +9882,11 @@
       <c r="B253" s="4">
         <v>44660</v>
       </c>
-      <c r="C253" s="3" t="s">
+      <c r="C253" s="5">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D253" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="D253" s="5">
-        <v>0.43055555555555558</v>
       </c>
       <c r="E253" s="3" t="s">
         <v>22</v>
@@ -9873,6 +9906,7 @@
       <c r="J253" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M253" s="3"/>
       <c r="N253" s="5"/>
     </row>
     <row r="254" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9882,11 +9916,11 @@
       <c r="B254" s="4">
         <v>44660</v>
       </c>
-      <c r="C254" s="3" t="s">
+      <c r="C254" s="5">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D254" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="D254" s="5">
-        <v>0.44444444444444442</v>
       </c>
       <c r="E254" s="3" t="s">
         <v>13</v>
@@ -9906,6 +9940,7 @@
       <c r="J254" s="24" t="s">
         <v>317</v>
       </c>
+      <c r="M254" s="3"/>
       <c r="N254" s="5"/>
     </row>
     <row r="255" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9915,11 +9950,11 @@
       <c r="B255" s="1">
         <v>44660</v>
       </c>
-      <c r="C255" t="s">
+      <c r="C255" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D255" t="s">
         <v>7</v>
-      </c>
-      <c r="D255" s="2">
-        <v>0.39583333333333331</v>
       </c>
       <c r="E255" t="s">
         <v>17</v>
@@ -9944,11 +9979,11 @@
       <c r="B256" s="1">
         <v>44660</v>
       </c>
-      <c r="C256" t="s">
+      <c r="C256" s="2">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="D256" t="s">
         <v>7</v>
-      </c>
-      <c r="D256" s="2">
-        <v>0.4236111111111111</v>
       </c>
       <c r="E256" t="s">
         <v>20</v>
@@ -9973,11 +10008,11 @@
       <c r="B257" s="1">
         <v>44660</v>
       </c>
-      <c r="C257" t="s">
+      <c r="C257" s="2">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="D257" t="s">
         <v>21</v>
-      </c>
-      <c r="D257" s="2">
-        <v>0.4513888888888889</v>
       </c>
       <c r="E257" t="s">
         <v>7</v>
@@ -10002,11 +10037,11 @@
       <c r="B258" s="1">
         <v>44660</v>
       </c>
-      <c r="C258" t="s">
+      <c r="C258" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D258" t="s">
         <v>136</v>
-      </c>
-      <c r="D258" s="2">
-        <v>0.375</v>
       </c>
       <c r="E258" t="s">
         <v>27</v>
@@ -10029,11 +10064,11 @@
       <c r="B259" s="1">
         <v>44660</v>
       </c>
-      <c r="C259" t="s">
+      <c r="C259" s="2">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D259" t="s">
         <v>138</v>
-      </c>
-      <c r="D259" s="2">
-        <v>0.44444444444444442</v>
       </c>
       <c r="E259" t="s">
         <v>34</v>
@@ -10056,11 +10091,11 @@
       <c r="B260" s="1">
         <v>44660</v>
       </c>
-      <c r="C260" t="s">
+      <c r="C260" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D260" t="s">
         <v>137</v>
-      </c>
-      <c r="D260" s="2">
-        <v>0.5</v>
       </c>
       <c r="E260" t="s">
         <v>30</v>
@@ -10083,11 +10118,11 @@
       <c r="B261" s="1">
         <v>44660</v>
       </c>
-      <c r="C261" t="s">
+      <c r="C261" s="2">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="D261" t="s">
         <v>139</v>
-      </c>
-      <c r="D261" s="2">
-        <v>0.52777777777777779</v>
       </c>
       <c r="E261" t="s">
         <v>36</v>
@@ -10110,11 +10145,11 @@
       <c r="B262" s="1">
         <v>44660</v>
       </c>
-      <c r="C262" t="s">
+      <c r="C262" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D262" t="s">
         <v>44</v>
-      </c>
-      <c r="D262" s="2">
-        <v>0.70833333333333337</v>
       </c>
       <c r="E262" t="s">
         <v>112</v>
@@ -10143,11 +10178,11 @@
       <c r="B263" s="1">
         <v>44660</v>
       </c>
-      <c r="C263" t="s">
+      <c r="C263" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D263" t="s">
         <v>40</v>
-      </c>
-      <c r="D263" s="2">
-        <v>0.75</v>
       </c>
       <c r="E263" t="s">
         <v>114</v>
@@ -10174,11 +10209,11 @@
       <c r="B264" s="1">
         <v>44660</v>
       </c>
-      <c r="C264" t="s">
+      <c r="C264" s="2">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="D264" t="s">
         <v>140</v>
-      </c>
-      <c r="D264" s="2">
-        <v>0.84722222222222221</v>
       </c>
       <c r="E264" t="s">
         <v>46</v>
@@ -10201,11 +10236,11 @@
       <c r="B265" s="1">
         <v>44671</v>
       </c>
-      <c r="C265" t="s">
+      <c r="C265" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="D265" t="s">
         <v>48</v>
-      </c>
-      <c r="D265" s="2">
-        <v>0.875</v>
       </c>
       <c r="E265" t="s">
         <v>133</v>
@@ -10234,11 +10269,11 @@
       <c r="B266" s="1">
         <v>44691</v>
       </c>
-      <c r="C266" t="s">
+      <c r="C266" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="D266" t="s">
         <v>141</v>
-      </c>
-      <c r="D266" s="2">
-        <v>0.875</v>
       </c>
       <c r="E266" t="s">
         <v>48</v>
@@ -10261,11 +10296,11 @@
       <c r="B267" s="30">
         <v>44513</v>
       </c>
-      <c r="C267" s="29" t="s">
+      <c r="C267" s="20">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D267" s="29" t="s">
         <v>34</v>
-      </c>
-      <c r="D267" s="20">
-        <v>0.66666666666666663</v>
       </c>
       <c r="E267" s="29" t="s">
         <v>101</v>
@@ -10288,6 +10323,7 @@
       <c r="K267" s="11" t="s">
         <v>319</v>
       </c>
+      <c r="M267" s="29"/>
       <c r="N267" s="20"/>
     </row>
     <row r="268" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -10297,11 +10333,11 @@
       <c r="B268" s="30">
         <v>44514</v>
       </c>
-      <c r="C268" s="29" t="s">
+      <c r="C268" s="20">
+        <v>0.4375</v>
+      </c>
+      <c r="D268" s="29" t="s">
         <v>103</v>
-      </c>
-      <c r="D268" s="20">
-        <v>0.4375</v>
       </c>
       <c r="E268" s="29" t="s">
         <v>40</v>
@@ -10318,18 +10354,20 @@
       <c r="K268" s="11" t="s">
         <v>321</v>
       </c>
+      <c r="M268" s="29"/>
       <c r="N268" s="20"/>
     </row>
     <row r="269" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B269" s="30"/>
-      <c r="C269" s="29"/>
-      <c r="D269" s="20"/>
+      <c r="C269" s="20"/>
+      <c r="D269" s="29"/>
       <c r="E269" s="29"/>
       <c r="F269" s="29"/>
       <c r="G269" s="29"/>
       <c r="H269" s="7"/>
       <c r="I269" s="7"/>
       <c r="J269" s="7"/>
+      <c r="M269" s="29"/>
       <c r="N269" s="20"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added comments and array with all errors
</commit_message>
<xml_diff>
--- a/wedstrijden.xlsx
+++ b/wedstrijden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\handbal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE8A3B9-5F4E-4A3D-8F12-80B149332D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688B0370-25C8-4C04-8635-1A8779EACA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2155,8 +2155,8 @@
   <dimension ref="A1:N269"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1:M1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>